<commit_message>
fixed api detected locations, name normalization, and master locations loading.
</commit_message>
<xml_diff>
--- a/assets/api_detected_locations.xlsx
+++ b/assets/api_detected_locations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B168"/>
+  <dimension ref="A1:B125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,1966 +484,1450 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>מוסך וצמיגים</t>
+          <t>טופ ויילס ספ בע"מ</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>32.186024,34.867836</t>
+          <t>32.605306,35.299672</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>טופ ויילס ספ בע"מ</t>
+          <t>מוסך אס</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>32.605306,35.299672</t>
+          <t>32.796643,35.689767</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>מוסך אס</t>
+          <t>צמיגי כהן מירו</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>32.796643,35.689767</t>
+          <t>32.766882,34.967053</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>צמיגי כהן מירו</t>
+          <t>מימון ובניו</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>32.766882,34.967053</t>
+          <t>32.511729,35.502029</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>מימון ובניו</t>
+          <t>מרכז שירות נ.ג בע"מ</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>32.511729,35.502029</t>
+          <t>32.189272,34.881159</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>מרכז שירות נ.ג בע"מ</t>
+          <t>צמיגי עוז</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>32.189272,34.881159</t>
+          <t>32.267628,34.993511</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>צמיגי עוז</t>
+          <t>צמיגי מצה בע"מ</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>32.267628,34.993511</t>
+          <t>32.792761,34.995336</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>צמיגי מצה בע"מ</t>
+          <t>ר.עולם הצמיגים בע"מ</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>32.792761,34.995336</t>
+          <t>31.829139,35.245637</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ר.עולם הצמיגים בע"מ</t>
+          <t>פנצ'רית סלע דוד</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>31.829139,35.245637</t>
+          <t>32.796567,34.983361</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>פנצ'רית סלע דוד</t>
+          <t>צמיג על רמה</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>32.796567,34.983361</t>
+          <t>32.028209,34.802593</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>צמיג על רמה</t>
+          <t>צמיגי פרויד בע"מ</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>32.028209,34.802593</t>
+          <t>32.323249,34.873417</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>צמיגי תמר</t>
+          <t>שרותי רכב מיכאלי יעקב ובניו</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>32.822823,35.059393</t>
+          <t>32.521941,34.992901</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>צמיגי פרויד בע"מ</t>
+          <t>פנצ'רית חניון משה</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>32.323249,34.873417</t>
+          <t>33.001898,35.097376</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>שרותי רכב מיכאלי יעקב ובניו</t>
+          <t>טיירדיל בע"מ</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>32.521941,34.992901</t>
+          <t>32.980490,35.542420</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>פנצ'רית חניון משה</t>
+          <t>פנצ'רית עבאדי</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>33.001898,35.097376</t>
+          <t>31.960770,34.876512</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>אברי דניאל ובניו</t>
+          <t>צמיגי דולפין</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>32.183636,34.880606</t>
+          <t>32.792761,34.995336</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>טיירדיל בע"מ</t>
+          <t>ג.ש.ר גולן שירותי רכב בע"מ</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>32.980490,35.542420</t>
+          <t>32.986934,35.708518</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>פנצ'רית עבאדי</t>
+          <t>אוטו טק בע"מ</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>31.960770,34.876512</t>
+          <t>32.794000,34.989600</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>צמיגי דולפין</t>
+          <t>בית הג'נטים והצמיגים</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>32.792761,34.995336</t>
+          <t>32.923530,35.080344</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>יריב לוי</t>
+          <t>מ.ח.צמיגי נהריה בע"מ</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>33.012090,35.440490</t>
+          <t>33.005860,35.094090</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ג.ש.ר גולן שירותי רכב בע"מ</t>
+          <t>אביב סוכנויות גלגלים בע"מ</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>32.986934,35.708518</t>
+          <t>32.601426,35.289751</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>אוטו טק בע"מ</t>
+          <t>מוסך רמת מגשימים</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>32.794000,34.989600</t>
+          <t>32.844029,35.807384</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>בית הג'נטים והצמיגים</t>
+          <t>המאסטרו א.ע.ייבוא ושיווק בע"מ</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>32.923530,35.080344</t>
+          <t>32.813048,35.059105</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>צמיגי רם</t>
+          <t>צמיגי אלבר</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>32.787820,35.028605</t>
+          <t>32.706861,35.173861</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>פנצ'רית העמק</t>
+          <t>4 ווילס 4 יו בע"מ</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>32.607430,35.292122</t>
+          <t>33.194459,35.572940</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>מ.ח.צמיגי נהריה בע"מ</t>
+          <t>צמיגי עודה</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>33.005860,35.094090</t>
+          <t>31.961063,34.807761</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>אביב סוכנויות גלגלים בע"מ</t>
+          <t>צמיגי יוסף אור יהודה בע"מ</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>32.601426,35.289751</t>
+          <t>32.036425,34.842884</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>מוסך רמת מגשימים</t>
+          <t>מולטי ריטייל גרופ-הילוך שישי ראשל"צ</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>32.844029,35.807384</t>
+          <t>31.977527,34.808252</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>המאסטרו א.ע.ייבוא ושיווק בע"מ</t>
+          <t>מולטי ריטייל גרופ-דיפו נתניה</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>32.813048,35.059105</t>
+          <t>32.310694,34.862344</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>צמיגי אלבר</t>
+          <t>צמיגי כרמל-קיסריה</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>32.706861,35.173861</t>
+          <t>31.784215,35.117210</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ח.איוב יבוא ושיווק צמיגים בע"מ</t>
+          <t>צמיגי רמת חן</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>32.792761,34.995336</t>
+          <t>32.058998,34.815227</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>4 ווילס 4 יו בע"מ</t>
+          <t>צמיגי אושיק</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>33.194459,35.572940</t>
+          <t>32.121447,34.803699</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>צמיגי עודה</t>
+          <t>ברק שירותי רחיצה</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>31.961063,34.807761</t>
+          <t>32.692764,34.940222</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>צמיגי יוסף אור יהודה בע"מ</t>
+          <t>מומנט אופנועים</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>32.036425,34.842884</t>
+          <t>31.750585,35.215673</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>ליעד ע.ה. שירותי רכב בע"מ</t>
+          <t>ברווז מוטורס</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>32.864774,35.279949</t>
+          <t>31.886629,34.781210</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>מולטי ריטייל גרופ-דוד לובינסקי ראשל"צ</t>
+          <t>צמיגי מגן בע"מ</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>31.950761,34.769037</t>
+          <t>32.137738,34.844184</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>מולטי ריטייל גרופ-הילוך שישי ראשל"צ</t>
+          <t>צמיגי טירה 1990 בע"מ</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>31.977527,34.808252</t>
+          <t>32.775683,34.967878</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>מולטי ריטייל גרופ-דיפו נתניה</t>
+          <t>צמיגי מושון בע"מ</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>32.310694,34.862344</t>
+          <t>32.199671,35.212911</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>צמיגי כרמל-קיסריה</t>
+          <t>צמיגי טיפ טופ יפו בע"מ</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>31.784215,35.117210</t>
+          <t>32.049533,34.764483</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>צמיגי רמת חן</t>
+          <t>צמיגי זיתוני חולון</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>32.058998,34.815227</t>
+          <t>32.008484,34.780119</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>דרור שרותי רכב בע"מ</t>
+          <t>צמיגי מטלון ותיקון צמיגים 2007 בע"מ</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>32.921645,35.311341</t>
+          <t>31.787546,35.178879</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>מרכז מקסיקו בע"מ</t>
+          <t>צמיגי רמת גן</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>32.322957,34.870299</t>
+          <t>32.195157,34.876308</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>צמיגי אושיק</t>
+          <t>צמיגי עוזנת בע"מ</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>32.121447,34.803699</t>
+          <t>32.327359,34.860597</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ברק שירותי רחיצה</t>
+          <t>צמיגי הירש רחובות בע"מ</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>32.692764,34.940222</t>
+          <t>31.885539,34.789352</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>פנצ'רית לונה 2010</t>
+          <t>צמיגי הרשת שי אדר בע"מ</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>32.807619,35.057422</t>
+          <t>32.023189,34.796457</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>מומנט אופנועים</t>
+          <t>דרייב קלין בע"מ</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>31.750585,35.215673</t>
+          <t>31.888478,34.781879</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>ברווז מוטורס</t>
+          <t>מולטי ריטייל גרופ-חיפה</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>31.886629,34.781210</t>
+          <t>32.792761,34.995336</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>צמיג ותקר</t>
+          <t>מולטי ריטייל גרופ-אשדוד</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>32.065611,34.787830</t>
+          <t>31.809016,34.655505</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>צמיגי מגן בע"מ</t>
+          <t>מולטי ריטייל גרופ-בילו</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>32.137738,34.844184</t>
+          <t>31.872097,34.819403</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>צמיגי טירה 1990 בע"מ</t>
+          <t>מולטי ריטייל גרופ-סינרמה</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>32.775683,34.967878</t>
+          <t>32.063929,34.791297</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>צמיגי יפו</t>
+          <t>צמיגי המהיר - יעקב</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>32.057122,34.757719</t>
+          <t>31.957286,34.897197</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>צמיגי יונתן כחלון</t>
+          <t>פנצ'רית הבילוי"ים</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>32.163295,34.809461</t>
+          <t>31.814560,34.779980</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>צמיגי מושון בע"מ</t>
+          <t>פנצ'רית הדרום בע"מ</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>32.199671,35.212911</t>
+          <t>31.248833,35.198232</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>צמיגי טיפ טופ יפו בע"מ</t>
+          <t>מולטי ריטייל גרופ-כ"ס</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>32.049533,34.764483</t>
+          <t>32.074578,34.805974</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>צמיגי זיתוני חולון</t>
+          <t>צמיגי זיתוני גבעתיים</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>32.008484,34.780119</t>
+          <t>32.071106,34.809852</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>גלגלי המגן</t>
+          <t>מולטי ריטייל גרופ-סגולה</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>32.197179,34.956413</t>
+          <t>32.101041,34.895807</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>צמיגי מטלון ותיקון צמיגים 2007 בע"מ</t>
+          <t>ח.חויו ובניו-סביון</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>31.787546,35.178879</t>
+          <t>32.590574,34.936472</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>צמיגי רמת גן</t>
+          <t>צמיגי המלך שלמה</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>32.195157,34.876308</t>
+          <t>31.808445,34.667116</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>מוסך סמדר</t>
+          <t>מולטי ריטייל גרופ-רגבה</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>32.083465,34.831047</t>
+          <t>32.973094,35.096904</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>צמיגי עוזנת בע"מ</t>
+          <t>צמיגי ורד א.ד 2002 בע"מ</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>32.327359,34.860597</t>
+          <t>32.018460,34.748167</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>מוסך צמיגי דובל</t>
+          <t>צמיגי ששון</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>31.928344,34.878259</t>
+          <t>32.098374,34.832515</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>צמיגי גיורא</t>
+          <t>צמיגי חנוכה</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>32.022467,34.864033</t>
+          <t>32.090108,34.838119</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>צמיגי הירש רחובות בע"מ</t>
+          <t>א.צמיגי המושבה בע"מ</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>31.885539,34.789352</t>
+          <t>31.802092,35.239517</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>צמיגי השפלה</t>
+          <t>צמיגי אורון</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>31.946700,34.890300</t>
+          <t>32.310694,34.862344</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>צמיגי הרשת שי אדר בע"מ</t>
+          <t>צמיגי אסף רחובות</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>32.023189,34.796457</t>
+          <t>31.822668,35.253867</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>דרייב קלין בע"מ</t>
+          <t>אבצמיג הנמל אשדוד בע"מ</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>31.888478,34.781879</t>
+          <t>31.791658,34.651074</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>מולטי ריטייל גרופ-חיפה</t>
+          <t>מרכז הצמיג ש.י. בע"מ</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>32.792761,34.995336</t>
+          <t>32.171739,34.825672</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>מולטי ריטייל גרופ-אשדוד</t>
+          <t>צמיגי מלי-מוסך 2001 בע"מ</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>31.809016,34.655505</t>
+          <t>32.319992,34.878531</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>מולטי ריטייל גרופ-בילו</t>
+          <t>גרין טייר</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>31.872097,34.819403</t>
+          <t>32.001204,34.763280</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>מולטי ריטייל גרופ-סינרמה</t>
+          <t>צמיגי צ'רלי חילו</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>32.063929,34.791297</t>
+          <t>32.107734,34.819964</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>צמיגי לביטל</t>
+          <t>צמיגי מקס שילת-סניף חדש</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>32.099514,34.895831</t>
+          <t>31.916670,35.016670</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>צמיגי המהיר - יעקב</t>
+          <t>אנטון חנניה-כוזרי</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>31.957286,34.897197</t>
+          <t>32.046875,34.762477</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>פנצ'רית הבילוי"ים</t>
+          <t>נחלים טופ טייר בע"מ</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>31.814560,34.779980</t>
+          <t>32.095980,34.774333</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>צמיגי מנשקו אשקלון</t>
+          <t>צמיגי ג'ינג'י בע"מ</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>31.669260,34.571490</t>
+          <t>32.020934,34.860824</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>כל צמיג דודי</t>
+          <t>מוסך עלי עבד אלקאדר בע"מ</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>32.065340,34.789086</t>
+          <t>31.854920,35.218710</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>פנצ'רית הדרום בע"מ</t>
+          <t>צמיגי מלאכי דארין</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>31.248833,35.198232</t>
+          <t>31.733160,34.754260</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>מולטי ריטייל גרופ-כ"ס</t>
+          <t>טכנולוגיות מרוצים (2002) בע"מ</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>32.074578,34.805974</t>
+          <t>32.067170,34.824745</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>צמיגי זיתוני גבעתיים</t>
+          <t>צמיגי מזור (אבן יהודה) בע"מ</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>32.071106,34.809852</t>
+          <t>32.280381,34.893250</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>מולטי ריטייל גרופ-סגולה</t>
+          <t>צמיגי החברים בע"מ</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>32.101041,34.895807</t>
+          <t>31.248833,35.198232</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>ח.חויו ובניו-סביון</t>
+          <t>צמיגי יוסי אוזן</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>32.590574,34.936472</t>
+          <t>31.733159,34.755513</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>צמיגי המלך שלמה</t>
+          <t>מ.מחסני צמיגים בע"מ</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>31.808445,34.667116</t>
+          <t>31.945204,34.878075</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>ל.מ.ש.מ נכסים בע"מ</t>
+          <t>מוסך ונטורה בע"מ</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>31.837794,34.683724</t>
+          <t>32.066408,34.789228</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>מולטי ריטייל גרופ-רגבה</t>
+          <t>צמיגי יבנה-זמורות הגפן בע"מ</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>32.973094,35.096904</t>
+          <t>31.866729,34.741793</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>צמיגי ורד א.ד 2002 בע"מ</t>
+          <t>היפר צמיג בע"מ</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>32.018460,34.748167</t>
+          <t>32.098181,34.896471</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>צמיגי ששון</t>
+          <t>פנצ'רית טיפ טופ בע"מ</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>32.098374,34.832515</t>
+          <t>32.015139,34.800425</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>צמיגי אבו אמיר</t>
+          <t>ח.חויו ובניו בע"מ</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>32.048936,34.769334</t>
+          <t>32.008484,34.780119</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>צמיגי חנוכה</t>
+          <t>פנצ'רית יוסי בע"מ</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>32.090108,34.838119</t>
+          <t>31.755957,34.989832</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>א.צמיגי המושבה בע"מ</t>
+          <t>חברת אלמסתקבל אלמשרק לצמיגים</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>31.802092,35.239517</t>
+          <t>31.776884,35.245249</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>צמיגי אורון</t>
+          <t>צמיגי דוידו מוטי</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>32.310694,34.862344</t>
+          <t>31.750898,35.207819</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>צמיגי אסף רחובות</t>
+          <t>אבי (ד.ע) שירותי רכב 24 שעות בע"מ</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>31.822668,35.253867</t>
+          <t>31.781280,35.249295</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>אבצמיג הנמל אשדוד בע"מ</t>
+          <t>ש.מ.אלנביל לצמיגים בע"מ</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>31.791658,34.651074</t>
+          <t>31.858601,35.215336</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>מרכז הצמיג ש.י. בע"מ</t>
+          <t>צמיגי שלומי נאסה בע"מ</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>32.171739,34.825672</t>
+          <t>32.177911,34.905656</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>צמיגי מלי-מוסך 2001 בע"מ</t>
+          <t>צמיגי בן כליפה</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>32.319992,34.878531</t>
+          <t>32.049272,34.798714</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>צמיגי בועז בע"מ</t>
+          <t>צמיגי רונדו מישור אדומים בע"מ</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>32.010787,34.746694</t>
+          <t>31.696076,34.570479</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>גרין טייר</t>
+          <t>זכי ואלון צמיגים ושרותי רכב בע"מ</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>32.001204,34.763280</t>
+          <t>31.792503,35.201657</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>צמיגי צ'רלי חילו</t>
+          <t>תמיר מרכז הצמיגים</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>32.107734,34.819964</t>
+          <t>31.226237,34.809557</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>צמיגי מקס שילת-סניף חדש</t>
+          <t>אשר צמיגים אלקובי</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>31.916670,35.016670</t>
+          <t>31.068012,35.007848</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>אנטון חנניה-כוזרי</t>
+          <t>צמיגי רפי מלכה בע"מ</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>32.046875,34.762477</t>
+          <t>31.238084,34.794545</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>נחלים טופ טייר בע"מ</t>
+          <t>ח.חויו ובניו בע"מ (תל אביב)</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>32.095980,34.774333</t>
+          <t>32.099594,34.782658</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>צמיגי עידן</t>
+          <t>ספייס קאר</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>31.975166,34.812732</t>
+          <t>32.009918,34.739188</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>צמיגי שואף</t>
+          <t>סולי אספקה טכנית ושירותי רכב בע"מ</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>31.262272,34.804363</t>
+          <t>31.863239,34.743120</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>צמיגי ג'ינג'י בע"מ</t>
+          <t>וחידי רמלה בע"מ</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>32.020934,34.860824</t>
+          <t>31.928344,34.878259</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>צמיגי אנטון חולון</t>
+          <t>צמיגי עומרי כחלון</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>32.009679,34.801882</t>
+          <t>32.174304,34.930966</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>מוסך עלי עבד אלקאדר בע"מ</t>
+          <t>צמיגי אנטון חנניה בע"מ</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>31.854920,35.218710</t>
+          <t>32.045852,34.752438</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>צמיגי מלאכי דארין</t>
+          <t>מוטי צמיגים</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>31.733160,34.754260</t>
+          <t>31.314100,34.620250</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>טכנולוגיות מרוצים (2002) בע"מ</t>
+          <t>הפנצ'ריה נ"צ</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>32.067170,34.824745</t>
+          <t>31.920741,34.794298</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>פנצ'רית אחים חילו</t>
+          <t>מוסך אריאל</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>32.048638,34.764526</t>
+          <t>32.860863,35.099385</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>צמיגי מזור (אבן יהודה) בע"מ</t>
+          <t>חצב נציגיויות בע"מ-כנות</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>32.280381,34.893250</t>
+          <t>32.471921,34.946694</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>צמיגי החברים בע"מ</t>
+          <t>אלת הצמיגים סחר והשקעות בע"מ</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>31.248833,35.198232</t>
+          <t>31.663407,34.599960</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>צמיגי יוסי אוזן</t>
+          <t>פנצ'ריית הגל</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>31.733159,34.755513</t>
+          <t>31.977527,34.808252</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>צמיגי סער</t>
+          <t>צמיגי שחר 2019 בע"מ</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>32.199671,35.212911</t>
+          <t>32.096376,34.836482</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>צמיגי מלאכי-רעננה</t>
+          <t>איובי אברהם עב' עפר בע"מ</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>32.194397,34.880223</t>
+          <t>31.682230,34.745240</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>מ.מחסני צמיגים בע"מ</t>
+          <t>טייר סנטר - פ"ת</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>31.945204,34.878075</t>
+          <t>32.090967,34.856886</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>צמיגי דוידו לירן</t>
+          <t>טייר סנטר - רמת אביב</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>32.104563,34.895062</t>
+          <t>32.104824,34.792871</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>מוסך ונטורה בע"מ</t>
+          <t>י. סגולה בע"מ</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>32.066408,34.789228</t>
+          <t>31.670900,34.779750</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>צמיגי רעננה שרון עוזי ואילן</t>
+          <t>צמיגי המוביל נור עיסאוי בע"מ</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>32.192266,34.881742</t>
+          <t>32.093309,34.885509</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>צמיגי יבנה-זמורות הגפן בע"מ</t>
+          <t>צמיגי איתן</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>31.866729,34.741793</t>
+          <t>31.246177,34.808709</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>צמיגי זיתוני ונעים</t>
+          <t>פסגת הצמיג</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>32.009775,34.749465</t>
+          <t>31.808795,35.240355</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>צמיגי פרץ ובניו</t>
+          <t>פנצ'ריית העיר בע"מ</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>31.986006,34.785113</t>
+          <t>31.756796,34.988601</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>היפר צמיג בע"מ</t>
+          <t>שירות לצמיגים מייק בן יוסף</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>32.098181,34.896471</t>
+          <t>32.053920,34.770991</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>פנצ'רית טיפ טופ בע"מ</t>
+          <t>דר' פנצ'ר</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
-        <is>
-          <t>32.015139,34.800425</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>צמיגי צמרת נתניה</t>
-        </is>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>32.310694,34.862344</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>ח.חויו ובניו בע"מ</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>32.008484,34.780119</t>
-        </is>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>פנצ'רית יוסי בע"מ</t>
-        </is>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>31.755957,34.989832</t>
-        </is>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>חברת אלמסתקבל אלמשרק לצמיגים</t>
-        </is>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>31.776884,35.245249</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>צמיגי דוידו מוטי</t>
-        </is>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>31.750898,35.207819</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t>אבי (ד.ע) שירותי רכב 24 שעות בע"מ</t>
-        </is>
-      </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>31.781280,35.249295</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>ש.מ.אלנביל לצמיגים בע"מ</t>
-        </is>
-      </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>31.858601,35.215336</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>צמיגי שלומי נאסה בע"מ</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>32.177911,34.905656</t>
-        </is>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>צמיגי שיר-קמ</t>
-        </is>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>31.747749,35.210602</t>
-        </is>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>צמיגי הרכב 2023 בע"מ</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>31.747780,35.209552</t>
-        </is>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>צמיגי בן כליפה</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>32.049272,34.798714</t>
-        </is>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>צמיגי רונדו מישור אדומים בע"מ</t>
-        </is>
-      </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>31.696076,34.570479</t>
-        </is>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="inlineStr">
-        <is>
-          <t>זכי ואלון צמיגים ושרותי רכב בע"מ</t>
-        </is>
-      </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>31.792503,35.201657</t>
-        </is>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" t="inlineStr">
-        <is>
-          <t>תמיר מרכז הצמיגים</t>
-        </is>
-      </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>31.226237,34.809557</t>
-        </is>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>אשר צמיגים אלקובי</t>
-        </is>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>31.068012,35.007848</t>
-        </is>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>צמיגי רפי מלכה בע"מ</t>
-        </is>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>31.238084,34.794545</t>
-        </is>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="inlineStr">
-        <is>
-          <t>ח.חויו ובניו בע"מ (תל אביב)</t>
-        </is>
-      </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>32.099594,34.782658</t>
-        </is>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>ספייס קאר</t>
-        </is>
-      </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>32.009918,34.739188</t>
-        </is>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>סולי אספקה טכנית ושירותי רכב בע"מ</t>
-        </is>
-      </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>31.863239,34.743120</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>וחידי רמלה בע"מ</t>
-        </is>
-      </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>31.928344,34.878259</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>צמיגי עומרי כחלון</t>
-        </is>
-      </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>32.174304,34.930966</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>צמיגי אנטון חנניה בע"מ</t>
-        </is>
-      </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>32.045852,34.752438</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>מוטי צמיגים</t>
-        </is>
-      </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>31.314100,34.620250</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>צמיגי ויקטור -רביד בע"מ</t>
-        </is>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>32.096621,34.849331</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="inlineStr">
-        <is>
-          <t>הפנצ'ריה נ"צ</t>
-        </is>
-      </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>31.920741,34.794298</t>
-        </is>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="inlineStr">
-        <is>
-          <t>מוסך אריאל</t>
-        </is>
-      </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>32.860863,35.099385</t>
-        </is>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="inlineStr">
-        <is>
-          <t>חצב נציגיויות בע"מ-כנות</t>
-        </is>
-      </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>32.471921,34.946694</t>
-        </is>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="inlineStr">
-        <is>
-          <t>אלת הצמיגים סחר והשקעות בע"מ</t>
-        </is>
-      </c>
-      <c r="B153" t="inlineStr">
-        <is>
-          <t>31.663407,34.599960</t>
-        </is>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>צמיגי הפלד בע"מ</t>
-        </is>
-      </c>
-      <c r="B154" t="inlineStr">
-        <is>
-          <t>32.023189,34.796457</t>
-        </is>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="inlineStr">
-        <is>
-          <t>פנצ'ריית הגל</t>
-        </is>
-      </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>31.977527,34.808252</t>
-        </is>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>פנצריית המחר</t>
-        </is>
-      </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>31.627591,34.585592</t>
-        </is>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="inlineStr">
-        <is>
-          <t>פנצ'ריית נתיבות</t>
-        </is>
-      </c>
-      <c r="B157" t="inlineStr">
-        <is>
-          <t>31.420078,34.600450</t>
-        </is>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="inlineStr">
-        <is>
-          <t>צמיגי שחר 2019 בע"מ</t>
-        </is>
-      </c>
-      <c r="B158" t="inlineStr">
-        <is>
-          <t>32.096376,34.836482</t>
-        </is>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>איובי אברהם עב' עפר בע"מ</t>
-        </is>
-      </c>
-      <c r="B159" t="inlineStr">
-        <is>
-          <t>31.682230,34.745240</t>
-        </is>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>טייר סנטר - פ"ת</t>
-        </is>
-      </c>
-      <c r="B160" t="inlineStr">
-        <is>
-          <t>32.090967,34.856886</t>
-        </is>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>טייר סנטר - רמת אביב</t>
-        </is>
-      </c>
-      <c r="B161" t="inlineStr">
-        <is>
-          <t>32.104824,34.792871</t>
-        </is>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>י. סגולה בע"מ</t>
-        </is>
-      </c>
-      <c r="B162" t="inlineStr">
-        <is>
-          <t>31.670900,34.779750</t>
-        </is>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>צמיגי המוביל נור עיסאוי בע"מ</t>
-        </is>
-      </c>
-      <c r="B163" t="inlineStr">
-        <is>
-          <t>32.093309,34.885509</t>
-        </is>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>צמיגי איתן</t>
-        </is>
-      </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>31.246177,34.808709</t>
-        </is>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>פסגת הצמיג</t>
-        </is>
-      </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>31.808795,35.240355</t>
-        </is>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>פנצ'ריית העיר בע"מ</t>
-        </is>
-      </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>31.756796,34.988601</t>
-        </is>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>שירות לצמיגים מייק בן יוסף</t>
-        </is>
-      </c>
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>32.053920,34.770991</t>
-        </is>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>דר' פנצ'ר</t>
-        </is>
-      </c>
-      <c r="B168" t="inlineStr">
         <is>
           <t>32.049539,34.953901</t>
         </is>

</xml_diff>

<commit_message>
switched from api to docker container for ors
</commit_message>
<xml_diff>
--- a/assets/api_detected_locations.xlsx
+++ b/assets/api_detected_locations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B125"/>
+  <dimension ref="A1:B484"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1933,6 +1933,4314 @@
         </is>
       </c>
     </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>א.ב.שוגן בע"מ</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>32.180235,34.918054</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>קוסטנדי גנטוס ובניו בע"מ</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>32.922276,35.081794</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>הפנצ'רייה של הקריה בע"מ</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>32.086219,34.783771</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>נגררי אבו מוך שיווק בע"מ</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>32.403106,35.050801</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>רוחצאומט  1986 בע"מ</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>32.789657,35.007866</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>הראל פנצ'ריה ושטיפת רכבים</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>33.052128,35.498807</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>איי.ג'י.אס.אגרו בע"מ</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>32.089254,34.812048</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>מוחמד מחמוד מוסא הובלות</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>32.977409,35.588354</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>אוטו פרו בע"מ</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>32.505841,35.047305</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>פנצ'ריית  ורחיצת חמודי</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>31.767207,35.224441</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>צמיגי גאד</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>32.028209,34.802593</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>צמיגי פרג 2024 בע"מ</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>32.450618,35.484785</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>חצב נציגויות בע"מ- ראש פינה</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>32.028209,34.802593</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>ראמי שירותי רכב</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>32.180235,34.918054</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>אלון יעקב הובלות בע"מ</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>32.986011,35.554083</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>סופר צמיג חדרה</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>32.447787,34.914428</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>מגאדלה עאיד מוסטפה</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>31.759553,35.219672</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>פופאי יבוא ושיווק צמיגים בע"מ</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>32.791937,35.531347</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>פנצריה אלעין</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>32.496286,35.098500</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>מחמוד.ע.אלחלים ובניו בע"מ</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>32.139558,34.959151</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>צמיגי יוסף בע"מ  (סניף יהוד)</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>32.027141,34.898820</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>הובלות אבו פנה בע"מ</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>32.180235,34.918054</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>סאלח אבו עביד בע"מ</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>32.706145,35.060734</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>מגדל החרמון בע"מ</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>33.262676,35.767928</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>קרדוש נצרת בע"מ</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>32.746415,35.281598</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>שירותי אוטובוסים מאוחדים נצרת יבוא בע"מ</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>32.758238,35.335589</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>מוסך עטיה יהודה</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>31.975998,34.882170</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>הפנצ'ריה של חיים שחר ביתן</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>32.968216,35.503177</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>צמיגי עלוש אברהים</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>32.703717,35.321868</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>מילואות-ת.דלק ושרותים בע"מ</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>32.216775,34.822412</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>ש.ר צמיגים ומצברים שובל אביב</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>32.780066,35.517715</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>קציר הצפון - הובלות סחר קש וחציר בע"מ</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>32.028209,34.802593</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>שטיפת רכב הלבנוני</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>33.001898,35.097376</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>החברה הצפונית לפינוי אשפה-פרץ חיים בע"מ</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>32.019045,34.841227</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>פנצ'ריית כפר כנא</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>32.798495,35.103304</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>טייסון צמיגים בע"מ</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>32.413870,35.021324</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>עוסמאן בן שרה הובלות בע"מ</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>32.798495,35.103304</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>מובילי נטופה מ.ע.ן בע"מ</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>32.532712,34.908322</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>ידידה סחר בע"מ</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>32.801454,35.069185</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>חצב נציגויות בע"מ - סניף צימו</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>32.450618,35.484785</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>בני משה ביטון ד. א. י. ש. בע"מ- בית שאן</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>31.781511,35.217024</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>אחים חרפאני בע"מ</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>33.200760,35.777989</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>צמיגי כרמל בע"מ</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>32.696543,35.052512</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>ח.קונפינו יבוא צמיגים בע"מ</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>31.746624,35.213931</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>צמיגי רונן יאיר</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>32.780066,35.517715</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>מוסך אבו חפיזה בע"מ</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>31.192304,34.841789</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>צמיגי O.K קתחודה</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>32.773251,35.044543</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>קרית הרכב ירכא בע"מ</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>31.854920,35.218710</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>עסלי רפקי ובניו בע"מ</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>31.192304,34.841789</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>צמיגי הגליל</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>33.016707,35.259739</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>עמית שרות התקר 2006 בע"מ</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>32.819327,34.997607</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>עדנאן מטר מכירת צמיגים</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>32.758238,35.335589</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>ע.מטר ואחיו בע"מ</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>31.854920,35.218710</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>ברק צמיגים בע"מ</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>31.785936,35.221741</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>פנצ'רית הצפון</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>32.798495,35.103304</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>צמיגי רמזי ובניו בע"מ</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>31.834088,34.681855</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>מוסך המרכז החדש בע"מ</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>32.960620,35.095419</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>א.א.שרותי רכב עפולה בע"מ</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>32.603829,35.298516</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>פנצ'רית לונה 2010 מוראד היתם</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>32.807619,35.057422</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>מוסך חלוצי בע"מ</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>32.804853,35.072857</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>צמיגי זחאלקה את זינאת בע"מ</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>32.180235,34.918054</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>פנצ'רית השלום</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>32.607430,35.292122</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>אריק צמיגים בע"מ</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>32.782155,34.976622</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>עותמאן חסן ובניו בע"מ</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>32.054678,34.804617</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>מטיילי דאניה בע"מ</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>31.265936,34.847616</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>ש.אחים זוהר לרכב בע"מ</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>32.798495,35.103304</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>פנצ'רית א.ר.ש</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>31.778240,35.230578</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>אזולאי בית משה בע"מ</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>32.019045,34.841227</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>א.ס.ק.ר הובלות ושיווק דלקים בע"מ</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>32.798495,35.103304</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>מרכז שירות א.ברק בע"מ</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>32.815143,35.060720</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>טייר ברהם</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>32.021724,34.797448</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>הסעות סולימאן בע"מ</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>32.180235,34.918054</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>מוסך חושי בע"מ</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>32.793011,35.040754</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>גדי גפן הובלות בע"מ</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>32.471755,34.969755</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>פ.מוזלבט חליל</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>32.180235,34.918054</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>מוסך קיבוץ כנרת</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>32.833740,35.061813</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>צוקים ר. 2015 בע"מ</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>32.863805,35.302318</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>צמיגי כבול</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>32.773251,35.044543</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>פנצ'רית ג'מאל</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>32.180235,34.918054</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>חסון ולאא צמיגים</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>32.163217,34.961133</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>צמיגי ויסאם רייא</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>32.163217,34.961133</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>צמיגי עבד אלחלים</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>32.028209,34.802593</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>צמיגי הצפון</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>32.933314,35.273731</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>א.ד.יבוא ושיווק צמיגים</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>32.790077,35.516279</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>המוביל שרותי מוסכים בע"מ</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>31.192304,34.841789</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>א.ביטון שירותי רכב בע"מ</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>32.139558,34.959151</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>פנצרית אבו גרור</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>32.107755,34.790275</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>סופר טראק י.ש. צמיגים בע"מ</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>31.785087,35.210391</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>צמיגי רוני בע"מ</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>31.973425,34.791984</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>צמיגי מג'ק</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>32.773251,35.044543</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>צמיגי אבו עזיז</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>32.716385,35.259434</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>אחים נעים יבוא ושיווק צמיגים בע"מ</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>32.028209,34.802593</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>צמיגי שקור</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>31.759144,34.998677</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>צמיגי ענאן חילו</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>32.450618,35.484785</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>טייר 4 יו בע"מ</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>32.564116,35.242224</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>המאסטרו א.ע יבוא ושיווק בע"מ</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>32.482073,34.943871</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>מוסך לחמי</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>32.019249,34.797620</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>פנצ'רית רביע אבו חפיזה</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>32.534917,35.171553</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>צמיגי אדמונד בגולן בע"מ</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>32.139558,34.959151</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>מ.ח.שדרוגים בע"מ</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>32.446027,34.915560</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>צמיגי יוסי בע"מ</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>31.767207,35.224441</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>מוסך סגול כרמיאל בע"מ</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>32.450618,35.484785</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>פנצ'רית הגולן</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>32.180235,34.918054</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>פנצ'רית וצמיגי אבו אלסאלח</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>32.868343,35.343268</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>צמיגי נעמן 2007</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>31.971973,34.761682</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>י.ו.צמיגים ושטיפה</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>32.773251,35.044543</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>חמודי מזגנים</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>32.868343,35.343268</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>מוסך מזרע א.ע.בע"מ</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>32.796643,35.689767</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>פנצ'ריית זערורה</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>32.803327,35.195999</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>פנצ'רית עבד עבוד</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>32.706854,35.265008</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>צמיגי זעיר זעיר</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>32.889209,35.238017</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>צמיגי יבור</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>32.037040,34.776415</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>א.ס.עבדולהאדי בע"מ</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>32.450618,35.484785</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>קיה צפון אילן נחימוב בע"מ</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>32.805007,35.055239</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>נ.א. צמיגים בע"מ</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>32.445945,34.911054</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>נצח תור בע"מ</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>32.180235,34.918054</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>צמיגי הצפון-ראש פינה</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>32.450618,35.484785</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>מוחמד שאמי</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>32.916364,35.125162</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>צמיגי אכסאל שלבי אחמד</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>32.180235,34.918054</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>פנצ'רית הגבעה</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>31.767207,35.224441</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>פנצ'ריית מעיליא-ח'ורי</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>31.778240,35.230578</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>טייר פרו תל חנן</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>32.777129,35.040632</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>ויסאם זאייד</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>32.450618,35.484785</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>צדוק אחזקה ושירותים בע"מ</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>32.019045,34.841227</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>צמיגי אבו חסן</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>32.706854,35.265008</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>ליאור הכל לרכב</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>32.960284,35.498750</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>צמיגי האלוף</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>32.767567,34.967656</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>אלמאז צמיגים בע"מ</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>32.704636,35.297185</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>אלחג' חלקי חילוף</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>32.854815,35.196680</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>עודה מאמון צמיגים</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>32.163217,34.961133</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>מוסך ופנצריית יוסף פדול</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>32.979582,35.333484</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>צמיגי ראמה ניקולא</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>32.180235,34.918054</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>א.ס.י אמפיר סחר ויבוא בע"מ</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>31.750585,35.215673</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>צימו צ'ק פוסט 1990</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>32.755356,35.061464</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>פנצ'רית עדנאן</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>32.862750,35.366381</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>א.אמיר סחר והפצה צמיגים בע"מ</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>32.505841,35.047305</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>פנצ'רית אדיב אבו עבדי</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>32.803327,35.195999</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>טכנו מנוע צפון בע"מ</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>31.975998,34.882170</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>מוסך נרקיס שרון את רוני בע"מ</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>32.194163,34.880735</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>TYRE SPEED</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>32.180235,34.918054</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>מולטי ריטייל גרופ-כל מוביל חיפה</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>32.450618,35.484785</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>מולטי ריטייל גרופ-צ'מפיון פ"ת</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>31.750859,35.213920</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>מולטי ריטייל גרופ-דנאל מוטורס כ"ס</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>32.139558,34.959151</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>קיבוץ משמר העמק אגש"ח בע"מ</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>32.611996,35.140562</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>מולטי רייטל גרופ-בני ברק</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>32.099592,34.828768</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>סבאג פאוזי בע"מ</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>31.854920,35.218710</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>טייר 4 יו בע"מ-קרע</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>32.505841,35.047305</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>עולם הרכב</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>32.633028,35.401886</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>טייר פוינט</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>32.803327,35.195999</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>הורן שירותי מוסך בע"מ</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>32.046554,34.869660</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>ויאם שיווק צמיגים בע"מ</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>32.984064,35.248787</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>צמיגי אירופה</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>32.755356,35.061464</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>צמיגי ויתקין</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>32.380323,34.882731</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>פרג אוניברסיטת הצמיג-סניף 3</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>32.534917,35.171553</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>פנצרית האחים</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>32.440953,34.909925</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>אבירון אופנועים</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>31.832481,34.673683</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>מוטוהייטק</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>31.813664,34.667678</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>י.ק.מוטוקלאס בע"מ</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>31.663407,34.599960</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>רפידו מוסך אופנועים</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>31.669700,34.600713</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>אלף אופנועים</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>32.461863,34.948124</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>ה.מ.ישראל בע"מ</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>31.604543,34.757505</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>מטרו מוטור שיווק (1981) בע"מ</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>32.166617,34.928168</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>המגרש</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>32.805007,35.055239</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>יאב</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>32.818629,34.996670</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>ניר ד"ר סייקל</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>32.805007,35.055239</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>סוזוקה ע.פ בע"מ</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>32.781607,35.035275</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>קטנועי אבי</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>32.801278,35.075851</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>מ.ג מאיר אקסטרים ונגררים בע"מ</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>32.779299,35.500918</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>YD MOTO</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>31.749982,35.214338</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>יוני אופנועים (ירושלים)</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>31.750492,35.215772</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>דראג אופנועים</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>31.785775,35.182708</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>מיסטר מוטו בע"מ</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>31.750585,35.215673</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>ביג בן- ביג</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>31.747838,35.209323</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>מוסך רמזור בע"מ</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>31.750492,35.215772</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>ד.מ.ד אופנועים (אדק'דק)</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>31.824870,35.227730</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>רק אופנועים</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>31.750585,35.215673</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>רועי מוטור</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>31.981085,34.765638</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>ניר מלול - סופר מוטו צפון</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>32.033640,34.849669</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>ש.ח. אופנועים</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>32.276787,34.858224</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>אופנועי האחים</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>31.635798,34.555246</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>דור אופנועים</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>32.048844,34.782469</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>בולי בייק</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>32.194693,34.884294</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>עמרם אופנועים וחלקים</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>31.749963,35.141489</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>מלכי שרותים טכניים</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>32.045764,34.789993</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>אדיר אופנועים</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>32.280381,34.893250</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>אקסטרים</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>32.320913,34.874430</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>מוסך HOLESHOT</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>33.003241,35.091790</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>מירו קרוס</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>32.767567,34.967656</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>מוסך הקטנוע רוזנר</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>33.001898,35.097376</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>אקסטרים מוטוספורט 1 בע"מ</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>31.779932,35.213532</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>אי.וי.מוטורס</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>31.750859,35.213920</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>אופנו בייק סנטר</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>32.180235,34.918054</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>טויוטה אוטופיה</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>31.888340,34.960893</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>צ'מפיון ירושלים</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>32.052717,34.770903</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>קליבר פתרונות טכניים</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>31.329171,34.651651</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>התותח אפנועים</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>31.961063,34.807761</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>טופ אר.אס בע"מ</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>31.774989,34.701294</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>טופ שופ אופנועים</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>32.773251,35.044543</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>שחם בוטיק אופנועים</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>31.778847,35.225786</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>ברמ מוטו סנטר</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>32.824143,34.992491</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>MOTO MS</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>32.781440,35.024204</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>אנדורו מוטו</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>32.532712,34.908322</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>א.מ.סייקל סוכנויות</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>32.634010,35.403998</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>ארז ניר סוכנויות</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>31.890353,34.786988</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>ברם מוטו סנטר</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>32.824143,34.992491</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>אופנוטרייד</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>32.318320,34.893605</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>ג'ורג'יניו מוטורס</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>32.028209,34.802593</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>המכונאי</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>31.863389,34.742527</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>מוטור שופ</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>32.704636,35.297185</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>ביסאן קסטרו מוטורס</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>32.949509,35.174243</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>די אנד אס מוטורס</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>31.784988,35.210374</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>מוטוגז</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>30.614095,35.184641</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>א.ע. שופ מוטורס 2022 בע"מ</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>31.971973,34.761682</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>מ.ג. יגמור מוטורס</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>31.856088,35.216314</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>אר מוטור</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>31.757498,35.218264</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>קוגול יוניטרייד מחסן לוד</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>31.949339,34.889317</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>צמיגי גלגלי העיר</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>31.975042,34.810956</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>זיתוני גבעתיים</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>32.088541,34.883662</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>י.ד.צמיגי טופ (2011) בע"מ</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>30.614095,35.184641</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>צמיגי העיר ראשון בע"מ</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>32.687340,35.422563</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>מרכז הצמיג ש.י. בע"מ-הסדנאות</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>32.161597,34.807131</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>פנצ'רית האור-רמת חן</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>32.048554,34.814926</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>סס טופ צמיגים בע"מ</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>31.563558,34.672081</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>עמיאל שיווק צמיגים בראשל"צ בע"מ</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>31.897055,34.800408</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>צמיגי רביע</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>32.761383,34.971551</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>צמיגי מוריס בית עובד</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>32.784567,35.031646</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>עודד רייכמן בע"מ</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>32.097206,34.825724</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>צמיגי מוריס</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>32.102931,34.897038</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>חיים וקנין שרותי רכב בע"מ</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>32.163217,34.961133</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>צמיגי אביעד</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>32.046638,34.790187</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>צמיגי בר רחובות בע"מ</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>32.151070,34.847113</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>יו.אס.אי.אי בע"מ</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>31.998810,34.946978</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>דרך צלחה שירותי הובלה בע"מ</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>31.652206,34.579598</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>מולטי ריטייל גרופ-ב"ש</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>31.194371,34.837706</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>מולטי ריטייל גרופ-ראשל"צ</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>32.141886,34.830791</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>מולטי ריטייל גרופ-ירושלים</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>31.747225,35.212499</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>מולטי ריטייל גרופ-נצרת</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>32.163217,34.961133</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>לה גראג' בר-קפה בע"מ</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>32.031743,34.853153</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>פנצ'רית עמיאל אשדוד בע"מ</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>31.834045,34.688455</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>שלב 1945 הובלות (2004) בע"מ</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>31.773929,34.629620</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>פאוור - טייר נס ציונה</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>32.155338,34.920541</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>מאיר מרכזי שירות שותפות מוגבלת</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>31.755555,35.212620</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>צמיגי דרור שילת בע"מ</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>32.019045,34.841227</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>צמיגי עמוס אשדוד בע"מ</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>31.811874,34.662521</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>צמיגי 2000</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>31.526474,34.596970</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>צמיגי מקס שילת בע"מ</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>32.019045,34.841227</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>מולטי ריטייל גרופ-בית שמש</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>31.755957,34.989832</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>טייר מאסטר ב.ג בע"מ-ליסינג</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>31.784215,35.117210</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>עמיאל שיווק-כלמוביל פ"ת</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>31.557766,34.546226</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>צמיגי אור</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>32.151070,34.847113</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>י.מ.צמיגים בע"מ</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>32.100120,34.828677</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>חצב סחר (1993) בע"מ</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>29.557397,34.954113</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>צמיגי זמר פלוס</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>32.362210,35.032513</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>רחיצה וצמיגים  עבד</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>32.603881,35.443679</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>מוסך י.פ. העוגן בע"מ</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>32.796643,35.689767</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>מולטי ריטייל גרופ-מבקעים</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>31.627488,34.582510</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>רן-שי שרותי הסעות בע"מ</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>32.163217,34.961133</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>צמיגי אחים ברנס אשדוד בע"מ</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>31.809919,34.666575</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>א.א בית הצמיג</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>32.139558,34.959151</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>צמיגי מירן</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>32.283414,34.860866</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>צמיגי שמעון כחלון בע"מ</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>32.160479,34.806955</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>ת.ג.ח</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>32.139558,34.959151</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>צמיגי ליגד בע"מ</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>32.047811,34.882122</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>צמיגי טל</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>32.165553,34.813406</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>TYRE CAR ת" א</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>32.074275,34.795528</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>צמיגי קחלון</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>31.982527,34.765084</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>צמיגי המהיר באר יעקב</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>31.946966,34.838993</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>מרכז הפרונט צמיגי התחנה</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>31.807623,34.664804</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>BEST DRIVE</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>32.162698,34.807924</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>ה.ג.ר המוביל גיבלי ראובן בע"מ</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>32.019045,34.841227</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>איתן הובלות ציוד כבד בע"מ</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>32.180235,34.918054</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>אל על - נתיבי אוויר לישראל</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>31.192304,34.841789</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>מובילי הורדים בע"מ</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>32.798495,35.103304</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>טיירו נעים בע"מ</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>32.088541,34.883662</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>סאלח חמיס ובניו בע"מ</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>32.055436,34.805472</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>יסמין הובלות ושיווק דבוריה בע</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>32.798495,35.103304</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>צמיגי ג'ו חולון</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>32.020682,34.805150</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>שירון(1989)י.ש.צמיגים בע"מ</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>32.097022,34.829235</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>תעשיות בית אל זכרון יעקב בע"מ</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>32.163217,34.961133</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>צמיגי המילניום מסחר ושר' בע"מ</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>31.665784,34.601137</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>יענקלה איתן גורן לחקלאי בע"מ</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>31.280566,34.443763</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>חברת י.א. אשכנזי הובלות מחצב ועבודות עפר בע"מ</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>31.975998,34.882170</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>צמיגי הפלד</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>32.023189,34.796457</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>מאיר דהן הובלות בע"מ</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>31.677567,34.596921</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>טייר סנטר ישיר בע"מ</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>32.090967,34.856886</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>הלסן חברה ליצור ושווק בע"מ</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>32.471200,34.972970</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>צמיגי לוד</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>31.946849,34.879864</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>אלעבידי למסחר ודלקים בע"מ</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>31.787184,35.215383</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>חברת צמיגי אלסלאמה בע"מ</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>31.927999,34.862347</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>מטיילי האחים דדון בע"מ</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>32.163217,34.961133</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>גי'.אר.אם סחר וצמיגים בע"מ</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>31.858601,35.215336</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>פנצ'רית טיפ טופ בע"מ-עטרות</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>31.858484,35.215449</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>ג'אזי שהאב</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>31.784992,35.236855</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>צמיגי ליאור 2020 בע"מ</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>31.750492,35.215772</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>מוסך הבירה בע"מ</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>31.659743,34.995688</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>טיפ טופ טיירס עטרות בע"מ</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>31.858484,35.215449</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>צמיגי הראל בע"מ</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>31.792463,35.144323</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>א.נ.ש סחר כללי</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>32.163217,34.961133</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>מוסך שרון מועלם</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>31.753295,34.996429</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>צמיגי אבו גוש</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>32.163217,34.961133</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>מקור הצמיג והפרונט בע"מ</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>32.033552,34.851439</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>צדיק צמיגים 1998 בע"מ</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>31.604981,34.773667</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>צמיגי רפי בע"מ</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>31.238084,34.794545</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>צמיגי האחים ברבי בע"מ</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>31.225747,34.809580</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>הפנצ'ריה הכתומה בע"מ</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>31.785936,35.221741</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>ליבוביץ מרכז הצמיגים בע"מ</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>32.163217,34.961133</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>פנצ'ריה אלקובי</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>32.028209,34.802593</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>אלנור תובלה בע"מ</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>32.798495,35.103304</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>צמיגי באר שבע</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>32.798495,35.103304</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>צמיג ותקר 89</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>31.854920,35.218710</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>טיולי נווה המדבר בע"מ</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>31.862441,35.220615</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>צמיגי א.ברבי בע"מ</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>31.225747,34.809580</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>חלפי השוק אוטו אאוטלט בע"מ</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>31.218097,34.810700</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>מוסך קלדרון באר-שבע בע"מ</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>31.227518,34.808264</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>מובילי צפון הנגב (בן זקן) בע"מ</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>31.319243,34.623672</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>מיי טיירס בע"מ</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>33.038364,35.194692</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>פנצ'רית טויטו דוד</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>31.423353,34.600095</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>צמיגי קידר בע"מ</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>31.223100,34.820208</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>חלפי השוק נתיבות</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>31.414595,34.591114</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>צמיגי ג'נסיס בע"מ</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>31.995072,34.764432</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>ל.א פיקס שירותי רכב בע"מ</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>32.062544,34.789326</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>ח.חויו ובניו בע"מ -הרצליה</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>32.171208,34.826985</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>צמיגי סופר טייר קריית גת בע"מ</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>31.603322,34.779509</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>צמיגי אנטון חנניה בע"מ -רחובות</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>31.888478,34.781879</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>א.ש. עדן בע"מ</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>31.890426,34.738461</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>צמיגי המחלף בע"מ</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>32.774549,35.407187</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>ברק בלס צמיגי יהוד שבזי 2</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>32.028203,34.894368</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>פנצ'ריית וספי נמר</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>32.966152,35.592775</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>ד.א אסיה תעשיות בע"מ</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>31.226551,34.807177</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>פנצ'ריית רבנו 148 בע"מ</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>31.826014,34.658552</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>צמיגי חביב בע"מ</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>31.759553,35.219672</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>צמיגי דרך אשקלון</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>31.666206,34.591622</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>חצב ניציגויות  בע"מ - נס ציונה</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>31.767207,35.224441</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>חצב נציגויות בע"מ- חולון</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>32.001232,34.801778</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>חצב נציגויות בע"מ- פתח תקווה</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>32.095724,34.858840</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>גיא ס.ל. שינוע בע"מ</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>31.223512,34.880824</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>א.נ איתם בע"מ</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>31.217089,34.816739</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>נפתלי ברוורמן תובלה בע"מ</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>32.067950,34.885418</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>מוסכי ורד בע"מ</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>32.282955,34.864958</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>צמיגי אדל</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>31.995242,34.751023</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>שטיפת האושר פנצ'ריה בע"מ</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>31.236692,34.796056</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>בן גנון</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>32.068716,34.778964</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>גור עוז טכנולוגיות רכב בע"מ</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>32.028209,34.802593</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>א.ס רכינות השפלה בע"מ</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>31.835181,34.687980</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>צמיגי באר שבע בע"מ</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>31.245744,34.792518</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>שירות צמיגים א.סלי</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>32.163217,34.961133</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>מוקד ארז דרום (2002) בע"מ</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>31.767207,35.224441</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>צמיגי אמצע הדרך</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>32.451936,34.908777</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>מנופי הרצל בע"מ</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>31.223598,34.811506</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>צמיגי אחים עבד</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>32.721723,35.353731</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>מוסך ה' עצמאות בע"מ</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>32.107402,34.938858</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>בן בן צמיגים</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>31.665784,34.601137</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>פנצ'ריית אחמד תורקי</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>32.139558,34.959151</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>י.ק. תחבורה פרימיום בע"מ</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>32.059754,34.847623</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>צמיגי תמיר</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>30.305548,34.787296</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>סטאר שירותי רכב בע"מ</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>32.037040,34.776415</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>עותמאן חסן ובניו בע"מ- סניף גלילות</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>32.054678,34.804617</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>פנצ'ריית רמלוד</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>31.929667,34.889113</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>חצב נציגויות בע"מ -ורד</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>32.320913,34.874430</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed bug in optimization tab
</commit_message>
<xml_diff>
--- a/assets/api_detected_locations.xlsx
+++ b/assets/api_detected_locations.xlsx
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>32.189272,34.881159</t>
+          <t>32.179540,34.908235</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>32.706861,35.173861</t>
+          <t>32.707298,35.173307</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>32.807619,35.057422</t>
+          <t>32.808325,35.060120</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>31.750585,35.215673</t>
+          <t>31.748498,35.214655</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>32.163295,34.809461</t>
+          <t>32.163351,34.809456</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>32.018460,34.748167</t>
+          <t>32.064156,34.854185</t>
         </is>
       </c>
     </row>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>31.945204,34.878075</t>
+          <t>31.942541,34.872538</t>
         </is>
       </c>
     </row>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>31.755957,34.989832</t>
+          <t>31.753295,34.996429</t>
         </is>
       </c>
     </row>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>31.750898,35.207819</t>
+          <t>31.749399,35.210830</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>31.858601,35.215336</t>
+          <t>31.857912,35.215438</t>
         </is>
       </c>
     </row>
@@ -2097,7 +2097,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>31.226237,34.809557</t>
+          <t>31.225747,34.809580</t>
         </is>
       </c>
     </row>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>31.068012,35.007848</t>
+          <t>31.068028,35.007787</t>
         </is>
       </c>
     </row>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>31.238084,34.794545</t>
+          <t>31.238529,34.795441</t>
         </is>
       </c>
     </row>
@@ -2157,7 +2157,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>31.863239,34.743120</t>
+          <t>31.863818,34.742477</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>31.928344,34.878259</t>
+          <t>31.928328,34.878378</t>
         </is>
       </c>
     </row>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>32.174304,34.930966</t>
+          <t>32.175827,34.926297</t>
         </is>
       </c>
     </row>
@@ -2193,7 +2193,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>32.045852,34.752438</t>
+          <t>32.045844,34.752383</t>
         </is>
       </c>
     </row>
@@ -2265,7 +2265,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>31.663407,34.599960</t>
+          <t>31.665784,34.601137</t>
         </is>
       </c>
     </row>
@@ -2313,7 +2313,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>31.420078,34.600450</t>
+          <t>31.419806,34.603236</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>32.093309,34.885509</t>
+          <t>32.093937,34.885592</t>
         </is>
       </c>
     </row>
@@ -2397,7 +2397,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>31.246177,34.808709</t>
+          <t>31.244467,34.807280</t>
         </is>
       </c>
     </row>
@@ -2421,7 +2421,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>31.756796,34.988601</t>
+          <t>31.757029,34.990864</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
changed solver strategy to Global Best and added time limit to config and ui added to ui "advanced settings" section "first solution strategy" and "solver time limit"
</commit_message>
<xml_diff>
--- a/assets/api_detected_locations.xlsx
+++ b/assets/api_detected_locations.xlsx
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>32.179540,34.908235</t>
+          <t>32.189272,34.881159</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>32.707298,35.173307</t>
+          <t>32.706861,35.173861</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>31.748498,35.214655</t>
+          <t>31.750585,35.215673</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>32.064156,34.854185</t>
+          <t>32.018460,34.748167</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>31.942541,34.872538</t>
+          <t>31.945204,34.878075</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>31.753295,34.996429</t>
+          <t>31.755957,34.989832</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>31.749399,35.210830</t>
+          <t>31.750898,35.207819</t>
         </is>
       </c>
     </row>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>31.857912,35.215438</t>
+          <t>31.858601,35.215336</t>
         </is>
       </c>
     </row>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>31.225747,34.809580</t>
+          <t>31.226237,34.809557</t>
         </is>
       </c>
     </row>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>31.068028,35.007787</t>
+          <t>31.068012,35.007848</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>31.238529,34.795441</t>
+          <t>31.238084,34.794545</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>31.863818,34.742477</t>
+          <t>31.863239,34.743120</t>
         </is>
       </c>
     </row>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>31.928328,34.878378</t>
+          <t>31.928344,34.878259</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>32.175827,34.926297</t>
+          <t>32.174304,34.930966</t>
         </is>
       </c>
     </row>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>32.045844,34.752383</t>
+          <t>32.045852,34.752438</t>
         </is>
       </c>
     </row>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>31.665784,34.601137</t>
+          <t>31.663407,34.599960</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>32.093937,34.885592</t>
+          <t>32.093309,34.885509</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>31.244467,34.807280</t>
+          <t>31.246177,34.808709</t>
         </is>
       </c>
     </row>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>31.757029,34.990864</t>
+          <t>31.756796,34.988601</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
revert to commit Enhance 'Optimization Tab and Add Static Routes Functionality' [ea88793]
</commit_message>
<xml_diff>
--- a/assets/api_detected_locations.xlsx
+++ b/assets/api_detected_locations.xlsx
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>32.189272,34.881159</t>
+          <t>32.179540,34.908235</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>32.706861,35.173861</t>
+          <t>32.707298,35.173307</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>31.750585,35.215673</t>
+          <t>31.748498,35.214655</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>32.018460,34.748167</t>
+          <t>32.064156,34.854185</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>31.945204,34.878075</t>
+          <t>31.942541,34.872538</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>31.755957,34.989832</t>
+          <t>31.753295,34.996429</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>31.750898,35.207819</t>
+          <t>31.749399,35.210830</t>
         </is>
       </c>
     </row>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>31.858601,35.215336</t>
+          <t>31.857912,35.215438</t>
         </is>
       </c>
     </row>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>31.226237,34.809557</t>
+          <t>31.225747,34.809580</t>
         </is>
       </c>
     </row>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>31.068012,35.007848</t>
+          <t>31.068028,35.007787</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>31.238084,34.794545</t>
+          <t>31.238529,34.795441</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>31.863239,34.743120</t>
+          <t>31.863818,34.742477</t>
         </is>
       </c>
     </row>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>31.928344,34.878259</t>
+          <t>31.928328,34.878378</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>32.174304,34.930966</t>
+          <t>32.175827,34.926297</t>
         </is>
       </c>
     </row>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>32.045852,34.752438</t>
+          <t>32.045844,34.752383</t>
         </is>
       </c>
     </row>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>31.663407,34.599960</t>
+          <t>31.665784,34.601137</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>32.093309,34.885509</t>
+          <t>32.093937,34.885592</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>31.246177,34.808709</t>
+          <t>31.244467,34.807280</t>
         </is>
       </c>
     </row>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>31.756796,34.988601</t>
+          <t>31.757029,34.990864</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
made the solver change to path most constrained arc. removed from ui and code the stress test tolerances
</commit_message>
<xml_diff>
--- a/assets/api_detected_locations.xlsx
+++ b/assets/api_detected_locations.xlsx
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>32.179540,34.908235</t>
+          <t>32.189272,34.881159</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>32.707298,35.173307</t>
+          <t>32.706861,35.173861</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>31.748498,35.214655</t>
+          <t>31.750585,35.215673</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>32.064156,34.854185</t>
+          <t>32.018460,34.748167</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>31.942541,34.872538</t>
+          <t>31.945204,34.878075</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>31.753295,34.996429</t>
+          <t>31.755957,34.989832</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>31.749399,35.210830</t>
+          <t>31.750898,35.207819</t>
         </is>
       </c>
     </row>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>31.857912,35.215438</t>
+          <t>31.858601,35.215336</t>
         </is>
       </c>
     </row>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>31.225747,34.809580</t>
+          <t>31.226237,34.809557</t>
         </is>
       </c>
     </row>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>31.068028,35.007787</t>
+          <t>31.068012,35.007848</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>31.238529,34.795441</t>
+          <t>31.238084,34.794545</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>31.863818,34.742477</t>
+          <t>31.863239,34.743120</t>
         </is>
       </c>
     </row>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>31.928328,34.878378</t>
+          <t>31.928344,34.878259</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>32.175827,34.926297</t>
+          <t>32.174304,34.930966</t>
         </is>
       </c>
     </row>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>32.045844,34.752383</t>
+          <t>32.045852,34.752438</t>
         </is>
       </c>
     </row>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>31.665784,34.601137</t>
+          <t>31.663407,34.599960</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>32.093937,34.885592</t>
+          <t>32.093309,34.885509</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>31.244467,34.807280</t>
+          <t>31.246177,34.808709</t>
         </is>
       </c>
     </row>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>31.757029,34.990864</t>
+          <t>31.756796,34.988601</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated versionl. last updated file that had logic. milestone push, this is the new version 1.0
</commit_message>
<xml_diff>
--- a/assets/api_detected_locations.xlsx
+++ b/assets/api_detected_locations.xlsx
@@ -1953,7 +1953,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>32.922285,35.081723</t>
+          <t>32.922276,35.081794</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>32.142049,34.960396</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>32.025841,34.898708</t>
+          <t>32.027141,34.898820</t>
         </is>
       </c>
     </row>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>32.779946,35.512493</t>
+          <t>32.780066,35.517715</t>
         </is>
       </c>
     </row>
@@ -2397,7 +2397,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>32.803420,35.068525</t>
+          <t>32.801454,35.069185</t>
         </is>
       </c>
     </row>
@@ -2469,7 +2469,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>32.779946,35.512493</t>
+          <t>32.780066,35.517715</t>
         </is>
       </c>
     </row>
@@ -2541,7 +2541,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>32.823809,34.991295</t>
+          <t>32.819327,34.997607</t>
         </is>
       </c>
     </row>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>32.600735,35.296222</t>
+          <t>32.603829,35.298516</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>32.808325,35.060120</t>
+          <t>32.807619,35.057422</t>
         </is>
       </c>
     </row>
@@ -2685,7 +2685,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>32.781952,34.976533</t>
+          <t>32.782155,34.976622</t>
         </is>
       </c>
     </row>
@@ -2769,7 +2769,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>32.816472,35.058426</t>
+          <t>32.815143,35.060720</t>
         </is>
       </c>
     </row>
@@ -2817,7 +2817,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>32.473092,34.968854</t>
+          <t>32.471755,34.969755</t>
         </is>
       </c>
     </row>
@@ -2889,7 +2889,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>32.209639,34.964653</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -2901,7 +2901,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>32.209639,34.964653</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>32.779301,35.522875</t>
+          <t>32.790077,35.516279</t>
         </is>
       </c>
     </row>
@@ -2961,7 +2961,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>32.142049,34.960396</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -3645,7 +3645,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -4041,7 +4041,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>31.748498,35.214655</t>
+          <t>31.750585,35.215673</t>
         </is>
       </c>
     </row>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>32.209639,34.964653</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -4773,7 +4773,7 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>32.209639,34.964653</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>31.753295,34.996429</t>
+          <t>31.755957,34.989832</t>
         </is>
       </c>
     </row>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -5073,7 +5073,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -5085,7 +5085,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>32.166162,34.810351</t>
+          <t>32.165553,34.813406</t>
         </is>
       </c>
     </row>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>31.992690,34.909264</t>
+          <t>31.982527,34.765084</t>
         </is>
       </c>
     </row>
@@ -5133,7 +5133,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>31.813664,34.667678</t>
+          <t>31.807623,34.664804</t>
         </is>
       </c>
     </row>
@@ -5205,7 +5205,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>32.054678,34.804617</t>
+          <t>32.055436,34.805472</t>
         </is>
       </c>
     </row>
@@ -5229,7 +5229,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>32.011816,34.796993</t>
+          <t>32.020682,34.805150</t>
         </is>
       </c>
     </row>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>31.937727,34.837262</t>
+          <t>32.097022,34.829235</t>
         </is>
       </c>
     </row>
@@ -5265,7 +5265,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>31.663407,34.599960</t>
+          <t>31.665784,34.601137</t>
         </is>
       </c>
     </row>
@@ -5313,7 +5313,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>31.675767,34.597809</t>
+          <t>31.677567,34.596921</t>
         </is>
       </c>
     </row>
@@ -5349,7 +5349,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>31.942541,34.872538</t>
+          <t>31.946849,34.879864</t>
         </is>
       </c>
     </row>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>31.857912,35.215438</t>
+          <t>31.858601,35.215336</t>
         </is>
       </c>
     </row>
@@ -5409,7 +5409,7 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>31.855315,35.221246</t>
+          <t>31.858484,35.215449</t>
         </is>
       </c>
     </row>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>31.750585,35.215673</t>
+          <t>31.750492,35.215772</t>
         </is>
       </c>
     </row>
@@ -5457,7 +5457,7 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>31.855315,35.221246</t>
+          <t>31.858484,35.215449</t>
         </is>
       </c>
     </row>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>31.792434,35.144275</t>
+          <t>31.792463,35.144323</t>
         </is>
       </c>
     </row>
@@ -5493,7 +5493,7 @@
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>31.755957,34.989832</t>
+          <t>31.753295,34.996429</t>
         </is>
       </c>
     </row>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>32.006200,34.743653</t>
+          <t>32.033552,34.851439</t>
         </is>
       </c>
     </row>
@@ -5553,7 +5553,7 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>31.226237,34.809557</t>
+          <t>31.225747,34.809580</t>
         </is>
       </c>
     </row>
@@ -5637,7 +5637,7 @@
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>31.860925,35.220821</t>
+          <t>31.862441,35.220615</t>
         </is>
       </c>
     </row>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>31.226237,34.809557</t>
+          <t>31.225747,34.809580</t>
         </is>
       </c>
     </row>
@@ -5721,7 +5721,7 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>31.222301,34.819116</t>
+          <t>31.223100,34.820208</t>
         </is>
       </c>
     </row>
@@ -5769,7 +5769,7 @@
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>32.167359,34.823770</t>
+          <t>32.171208,34.826985</t>
         </is>
       </c>
     </row>
@@ -5853,7 +5853,7 @@
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>31.226727,34.804803</t>
+          <t>31.226551,34.807177</t>
         </is>
       </c>
     </row>
@@ -5865,7 +5865,7 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>31.828293,34.662887</t>
+          <t>31.826014,34.658552</t>
         </is>
       </c>
     </row>
@@ -5889,7 +5889,7 @@
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>31.666065,34.584567</t>
+          <t>31.666206,34.591622</t>
         </is>
       </c>
     </row>
@@ -5913,7 +5913,7 @@
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>32.008568,34.807885</t>
+          <t>32.001232,34.801778</t>
         </is>
       </c>
     </row>
@@ -5925,7 +5925,7 @@
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>32.095945,34.859010</t>
+          <t>32.095724,34.858840</t>
         </is>
       </c>
     </row>
@@ -5937,7 +5937,7 @@
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>31.222537,34.880798</t>
+          <t>31.223512,34.880824</t>
         </is>
       </c>
     </row>
@@ -5949,7 +5949,7 @@
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>31.220502,34.815623</t>
+          <t>31.217089,34.816739</t>
         </is>
       </c>
     </row>
@@ -5997,7 +5997,7 @@
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>31.237729,34.793597</t>
+          <t>31.236692,34.796056</t>
         </is>
       </c>
     </row>
@@ -6009,7 +6009,7 @@
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>32.159475,34.836814</t>
+          <t>32.068716,34.778964</t>
         </is>
       </c>
     </row>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>32.108556,34.939938</t>
+          <t>32.107402,34.938858</t>
         </is>
       </c>
     </row>
@@ -6129,7 +6129,7 @@
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>31.663407,34.599960</t>
+          <t>31.665784,34.601137</t>
         </is>
       </c>
     </row>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -6225,7 +6225,7 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>31.526474,34.596970</t>
+          <t>32.047811,34.882122</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
local commit before file merge
</commit_message>
<xml_diff>
--- a/assets/api_detected_locations.xlsx
+++ b/assets/api_detected_locations.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>32.766882,34.967053</t>
+          <t>32.767884,34.966961</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>32.511729,35.502029</t>
+          <t>33.084756,35.112133</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>32.267628,34.993511</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>32.792761,34.995336</t>
+          <t>32.267628,34.993511</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>32.980490,35.542420</t>
+          <t>31.854920,35.218710</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>31.960770,34.876512</t>
+          <t>32.019045,34.841227</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>32.986934,35.708518</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>33.005860,35.094090</t>
+          <t>32.773251,35.044543</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>32.601426,35.289751</t>
+          <t>32.606459,35.290914</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>33.194459,35.572940</t>
+          <t>31.854920,35.218710</t>
         </is>
       </c>
     </row>
@@ -789,7 +789,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>31.961063,34.807761</t>
+          <t>31.961622,34.807607</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>32.036425,34.842884</t>
+          <t>32.035964,34.845985</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>31.977527,34.808252</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>31.784215,35.117210</t>
+          <t>31.767207,35.224441</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>32.058998,34.815227</t>
+          <t>32.052244,34.797643</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>32.121447,34.803699</t>
+          <t>32.047035,34.899314</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>32.692764,34.940222</t>
+          <t>31.818922,35.194455</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>32.775683,34.967878</t>
+          <t>32.234686,34.954455</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>32.199671,35.212911</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -945,7 +945,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>32.049533,34.764483</t>
+          <t>32.049544,34.764454</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>32.792761,34.995336</t>
+          <t>32.037040,34.776415</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>31.814560,34.779980</t>
+          <t>32.081982,34.816659</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>31.248833,35.198232</t>
+          <t>32.028209,34.802593</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>32.074578,34.805974</t>
+          <t>33.132610,35.690627</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>32.590574,34.936472</t>
+          <t>31.767207,35.224441</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>32.018460,34.748167</t>
+          <t>32.064156,34.854185</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>31.822668,35.253867</t>
+          <t>32.149836,34.846582</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>31.791658,34.651074</t>
+          <t>32.006200,34.743653</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>31.916670,35.016670</t>
+          <t>32.037040,34.776415</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>32.095980,34.774333</t>
+          <t>31.818922,35.194455</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>31.248833,35.198232</t>
+          <t>32.028209,34.802593</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>31.945204,34.878075</t>
+          <t>31.942541,34.872538</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>32.098181,34.896471</t>
+          <t>32.097875,34.896155</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>31.750898,35.207819</t>
+          <t>31.746015,35.213772</t>
         </is>
       </c>
     </row>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>32.177911,34.905656</t>
+          <t>31.194371,34.837706</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>32.049272,34.798714</t>
+          <t>31.748475,35.212194</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>32.009918,34.739188</t>
+          <t>32.174844,34.814576</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>31.314100,34.620250</t>
+          <t>31.785936,35.221741</t>
         </is>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>32.860863,35.099385</t>
+          <t>31.785077,34.693905</t>
         </is>
       </c>
     </row>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>31.977527,34.808252</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>31.682230,34.745240</t>
+          <t>31.975998,34.882170</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>31.670900,34.779750</t>
+          <t>31.669726,34.779153</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>32.093309,34.885509</t>
+          <t>32.090535,34.885715</t>
         </is>
       </c>
     </row>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>32.447787,34.914428</t>
+          <t>32.063762,34.785644</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>32.696543,35.052512</t>
+          <t>31.767207,35.224441</t>
         </is>
       </c>
     </row>
@@ -2457,7 +2457,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>31.746624,35.213931</t>
+          <t>31.747674,35.214435</t>
         </is>
       </c>
     </row>
@@ -2541,7 +2541,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>32.819327,34.997607</t>
+          <t>32.823809,34.991295</t>
         </is>
       </c>
     </row>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>32.603829,35.298516</t>
+          <t>31.788356,35.213514</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>32.807619,35.057422</t>
+          <t>32.808325,35.060120</t>
         </is>
       </c>
     </row>
@@ -2649,7 +2649,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>32.804853,35.072857</t>
+          <t>32.806452,35.070911</t>
         </is>
       </c>
     </row>
@@ -2673,7 +2673,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>32.607430,35.292122</t>
+          <t>32.607513,35.292171</t>
         </is>
       </c>
     </row>
@@ -2685,7 +2685,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>32.782155,34.976622</t>
+          <t>32.787600,34.971328</t>
         </is>
       </c>
     </row>
@@ -2697,7 +2697,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>32.054678,34.804617</t>
+          <t>32.055436,34.805472</t>
         </is>
       </c>
     </row>
@@ -2769,7 +2769,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>32.815143,35.060720</t>
+          <t>32.818155,35.055460</t>
         </is>
       </c>
     </row>
@@ -2817,7 +2817,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>32.471755,34.969755</t>
+          <t>32.468029,34.974133</t>
         </is>
       </c>
     </row>
@@ -2889,7 +2889,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.209639,34.964653</t>
         </is>
       </c>
     </row>
@@ -2901,7 +2901,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.209639,34.964653</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>32.790077,35.516279</t>
+          <t>32.786982,35.518669</t>
         </is>
       </c>
     </row>
@@ -2961,7 +2961,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.142049,34.960396</t>
         </is>
       </c>
     </row>
@@ -2985,7 +2985,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>31.785087,35.210391</t>
+          <t>31.784988,35.210374</t>
         </is>
       </c>
     </row>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.142049,34.960396</t>
         </is>
       </c>
     </row>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>32.916364,35.125162</t>
+          <t>32.927663,35.151740</t>
         </is>
       </c>
     </row>
@@ -3393,7 +3393,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>32.777129,35.040632</t>
+          <t>32.777112,35.040416</t>
         </is>
       </c>
     </row>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>32.854815,35.196680</t>
+          <t>32.634010,35.403998</t>
         </is>
       </c>
     </row>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.267628,34.993511</t>
         </is>
       </c>
     </row>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>31.750585,35.215673</t>
+          <t>31.748498,35.214655</t>
         </is>
       </c>
     </row>
@@ -3633,7 +3633,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>31.750859,35.213920</t>
+          <t>31.750030,35.218672</t>
         </is>
       </c>
     </row>
@@ -3645,7 +3645,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.142049,34.960396</t>
         </is>
       </c>
     </row>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>32.099592,34.828768</t>
+          <t>32.099723,34.828750</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>32.046554,34.869660</t>
+          <t>32.047831,34.870851</t>
         </is>
       </c>
     </row>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>32.984064,35.248787</t>
+          <t>32.983671,35.251911</t>
         </is>
       </c>
     </row>
@@ -3813,7 +3813,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>31.813664,34.667678</t>
+          <t>31.818001,34.669804</t>
         </is>
       </c>
     </row>
@@ -3825,7 +3825,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>31.663407,34.599960</t>
+          <t>31.667321,34.601532</t>
         </is>
       </c>
     </row>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>32.818629,34.996670</t>
+          <t>32.830002,34.970337</t>
         </is>
       </c>
     </row>
@@ -3969,7 +3969,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>31.750492,35.215772</t>
+          <t>31.748475,35.212194</t>
         </is>
       </c>
     </row>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>31.785775,35.182708</t>
+          <t>31.785263,35.186530</t>
         </is>
       </c>
     </row>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>31.750585,35.215673</t>
+          <t>31.748498,35.214655</t>
         </is>
       </c>
     </row>
@@ -4017,7 +4017,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>31.750492,35.215772</t>
+          <t>31.748475,35.212194</t>
         </is>
       </c>
     </row>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>32.194693,34.884294</t>
+          <t>32.193962,34.884145</t>
         </is>
       </c>
     </row>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>31.749963,35.141489</t>
+          <t>31.781986,35.164617</t>
         </is>
       </c>
     </row>
@@ -4173,7 +4173,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>33.003241,35.091790</t>
+          <t>33.003303,35.091469</t>
         </is>
       </c>
     </row>
@@ -4221,7 +4221,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>31.750859,35.213920</t>
+          <t>31.750030,35.218672</t>
         </is>
       </c>
     </row>
@@ -4449,7 +4449,7 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>32.949509,35.174243</t>
+          <t>32.956311,35.211352</t>
         </is>
       </c>
     </row>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>31.784988,35.210374</t>
+          <t>31.785087,35.210391</t>
         </is>
       </c>
     </row>
@@ -4509,7 +4509,7 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>31.757498,35.218264</t>
+          <t>31.758017,35.215239</t>
         </is>
       </c>
     </row>
@@ -4617,7 +4617,7 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>31.897055,34.800408</t>
+          <t>31.893720,34.803882</t>
         </is>
       </c>
     </row>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.142049,34.960396</t>
         </is>
       </c>
     </row>
@@ -4701,7 +4701,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>32.151070,34.847113</t>
+          <t>32.153195,34.846595</t>
         </is>
       </c>
     </row>
@@ -4725,7 +4725,7 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>31.652206,34.579598</t>
+          <t>33.230371,35.639263</t>
         </is>
       </c>
     </row>
@@ -4761,7 +4761,7 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>31.747225,35.212499</t>
+          <t>31.749399,35.210830</t>
         </is>
       </c>
     </row>
@@ -4809,7 +4809,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>31.773929,34.629620</t>
+          <t>32.798495,35.103304</t>
         </is>
       </c>
     </row>
@@ -4905,7 +4905,7 @@
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>31.784215,35.117210</t>
+          <t>31.767207,35.224441</t>
         </is>
       </c>
     </row>
@@ -4929,7 +4929,7 @@
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>32.151070,34.847113</t>
+          <t>32.149836,34.846582</t>
         </is>
       </c>
     </row>
@@ -4941,7 +4941,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>32.100120,34.828677</t>
+          <t>32.188320,34.866618</t>
         </is>
       </c>
     </row>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.267628,34.993511</t>
         </is>
       </c>
     </row>
@@ -5073,7 +5073,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.267628,34.993511</t>
         </is>
       </c>
     </row>
@@ -5085,7 +5085,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>32.165553,34.813406</t>
+          <t>32.166162,34.810351</t>
         </is>
       </c>
     </row>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>31.982527,34.765084</t>
+          <t>31.992690,34.909264</t>
         </is>
       </c>
     </row>
@@ -5133,7 +5133,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>31.807623,34.664804</t>
+          <t>32.189272,34.881159</t>
         </is>
       </c>
     </row>
@@ -5205,7 +5205,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>32.055436,34.805472</t>
+          <t>32.054678,34.804617</t>
         </is>
       </c>
     </row>
@@ -5229,7 +5229,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>32.020682,34.805150</t>
+          <t>31.785936,35.221741</t>
         </is>
       </c>
     </row>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>32.097022,34.829235</t>
+          <t>31.937727,34.837262</t>
         </is>
       </c>
     </row>
@@ -5265,7 +5265,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>31.665784,34.601137</t>
+          <t>31.663407,34.599960</t>
         </is>
       </c>
     </row>
@@ -5313,7 +5313,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>31.677567,34.596921</t>
+          <t>31.675767,34.597809</t>
         </is>
       </c>
     </row>
@@ -5349,7 +5349,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>31.946849,34.879864</t>
+          <t>31.942541,34.872538</t>
         </is>
       </c>
     </row>
@@ -5409,7 +5409,7 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>31.858484,35.215449</t>
+          <t>31.855315,35.221246</t>
         </is>
       </c>
     </row>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>31.750492,35.215772</t>
+          <t>31.750585,35.215673</t>
         </is>
       </c>
     </row>
@@ -5457,7 +5457,7 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>31.858484,35.215449</t>
+          <t>31.855315,35.221246</t>
         </is>
       </c>
     </row>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>31.792463,35.144323</t>
+          <t>32.086358,34.802173</t>
         </is>
       </c>
     </row>
@@ -5481,7 +5481,7 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.142049,34.960396</t>
         </is>
       </c>
     </row>
@@ -5505,7 +5505,7 @@
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.142049,34.960396</t>
         </is>
       </c>
     </row>
@@ -5541,7 +5541,7 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>31.238529,34.795441</t>
+          <t>31.238084,34.794545</t>
         </is>
       </c>
     </row>
@@ -5577,7 +5577,7 @@
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.142049,34.960396</t>
         </is>
       </c>
     </row>
@@ -5685,7 +5685,7 @@
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>31.319243,34.623672</t>
+          <t>31.669700,34.600713</t>
         </is>
       </c>
     </row>
@@ -5865,7 +5865,7 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>31.826014,34.658552</t>
+          <t>31.828282,34.663017</t>
         </is>
       </c>
     </row>
@@ -6057,7 +6057,7 @@
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.142049,34.960396</t>
         </is>
       </c>
     </row>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.209639,34.964653</t>
         </is>
       </c>
     </row>
@@ -6189,7 +6189,7 @@
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>32.054678,34.804617</t>
+          <t>32.055436,34.805472</t>
         </is>
       </c>
     </row>
@@ -6225,7 +6225,7 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>32.047811,34.882122</t>
+          <t>31.526474,34.596970</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated version - before ui fixes & merge
</commit_message>
<xml_diff>
--- a/assets/api_detected_locations.xlsx
+++ b/assets/api_detected_locations.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>32.766882,34.967053</t>
+          <t>32.767884,34.966961</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>32.511729,35.502029</t>
+          <t>33.084756,35.112133</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>32.267628,34.993511</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>32.792761,34.995336</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>32.980490,35.542420</t>
+          <t>31.854920,35.218710</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>31.960770,34.876512</t>
+          <t>32.019045,34.841227</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>32.986934,35.708518</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>33.005860,35.094090</t>
+          <t>32.773251,35.044543</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>32.601426,35.289751</t>
+          <t>32.606459,35.290914</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>32.706861,35.173861</t>
+          <t>32.707298,35.173307</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>33.194459,35.572940</t>
+          <t>31.854920,35.218710</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>31.977527,34.808252</t>
+          <t>32.197179,34.956413</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>31.784215,35.117210</t>
+          <t>31.767207,35.224441</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>32.058998,34.815227</t>
+          <t>32.052244,34.797643</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>32.121447,34.803699</t>
+          <t>32.047035,34.899314</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>32.692764,34.940222</t>
+          <t>31.790191,35.198620</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>31.750585,35.215673</t>
+          <t>31.748498,35.214655</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>32.775683,34.967878</t>
+          <t>32.234686,34.954455</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>32.199671,35.212911</t>
+          <t>32.197179,34.956413</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>31.885539,34.789352</t>
+          <t>31.886326,34.786696</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>32.023189,34.796457</t>
+          <t>32.020531,34.799529</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>32.792761,34.995336</t>
+          <t>32.037040,34.776415</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>31.814560,34.779980</t>
+          <t>32.081982,34.816659</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>31.248833,35.198232</t>
+          <t>32.028209,34.802593</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>32.074578,34.805974</t>
+          <t>33.132610,35.690627</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>32.590574,34.936472</t>
+          <t>31.767207,35.224441</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>32.018460,34.748167</t>
+          <t>32.064156,34.854185</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>31.822668,35.253867</t>
+          <t>32.151070,34.847113</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>31.791658,34.651074</t>
+          <t>32.006200,34.743653</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>31.916670,35.016670</t>
+          <t>32.037040,34.776415</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>32.095980,34.774333</t>
+          <t>31.818922,35.194455</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>31.248833,35.198232</t>
+          <t>32.028209,34.802593</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>31.945204,34.878075</t>
+          <t>31.942541,34.872538</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>32.098181,34.896471</t>
+          <t>32.097875,34.896155</t>
         </is>
       </c>
     </row>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>32.177911,34.905656</t>
+          <t>31.194371,34.837706</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>32.049272,34.798714</t>
+          <t>31.748475,35.212194</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>32.009918,34.739188</t>
+          <t>32.174844,34.814576</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>31.314100,34.620250</t>
+          <t>31.785936,35.221741</t>
         </is>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>32.860863,35.099385</t>
+          <t>31.785077,34.693905</t>
         </is>
       </c>
     </row>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>31.977527,34.808252</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>31.682230,34.745240</t>
+          <t>31.975998,34.882170</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>31.670900,34.779750</t>
+          <t>31.669726,34.779153</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>32.093309,34.885509</t>
+          <t>32.090535,34.885715</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>32.807619,35.057422</t>
+          <t>32.783385,35.036378</t>
         </is>
       </c>
     </row>
@@ -2961,7 +2961,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>32.916364,35.125162</t>
+          <t>32.927663,35.151740</t>
         </is>
       </c>
     </row>
@@ -3393,7 +3393,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>32.777129,35.040632</t>
+          <t>32.777112,35.040416</t>
         </is>
       </c>
     </row>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.209639,34.964653</t>
         </is>
       </c>
     </row>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>31.750585,35.215673</t>
+          <t>31.748475,35.212194</t>
         </is>
       </c>
     </row>
@@ -3633,7 +3633,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>31.750859,35.213920</t>
+          <t>31.750030,35.218672</t>
         </is>
       </c>
     </row>
@@ -3645,7 +3645,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.197179,34.956413</t>
         </is>
       </c>
     </row>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>32.099592,34.828768</t>
+          <t>32.099723,34.828750</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>32.046554,34.869660</t>
+          <t>32.047831,34.870851</t>
         </is>
       </c>
     </row>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>32.984064,35.248787</t>
+          <t>32.983671,35.251911</t>
         </is>
       </c>
     </row>
@@ -3813,7 +3813,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>31.813664,34.667678</t>
+          <t>31.818001,34.669804</t>
         </is>
       </c>
     </row>
@@ -3825,7 +3825,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>31.663407,34.599960</t>
+          <t>31.667321,34.601532</t>
         </is>
       </c>
     </row>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>32.818629,34.996670</t>
+          <t>32.830002,34.970337</t>
         </is>
       </c>
     </row>
@@ -3969,7 +3969,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>31.750492,35.215772</t>
+          <t>31.748475,35.212194</t>
         </is>
       </c>
     </row>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>31.785775,35.182708</t>
+          <t>31.785263,35.186530</t>
         </is>
       </c>
     </row>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>31.750585,35.215673</t>
+          <t>31.748475,35.212194</t>
         </is>
       </c>
     </row>
@@ -4017,7 +4017,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>31.750492,35.215772</t>
+          <t>31.748475,35.212194</t>
         </is>
       </c>
     </row>
@@ -4041,7 +4041,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>31.750585,35.215673</t>
+          <t>31.748498,35.214655</t>
         </is>
       </c>
     </row>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>32.194693,34.884294</t>
+          <t>32.193962,34.884145</t>
         </is>
       </c>
     </row>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>31.749963,35.141489</t>
+          <t>31.781986,35.164617</t>
         </is>
       </c>
     </row>
@@ -4173,7 +4173,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>33.003241,35.091790</t>
+          <t>33.003303,35.091469</t>
         </is>
       </c>
     </row>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>31.784988,35.210374</t>
+          <t>31.785087,35.210391</t>
         </is>
       </c>
     </row>
@@ -4497,7 +4497,7 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>31.856088,35.216314</t>
+          <t>31.850998,35.218030</t>
         </is>
       </c>
     </row>
@@ -4509,7 +4509,7 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>31.757498,35.218264</t>
+          <t>31.757946,35.215351</t>
         </is>
       </c>
     </row>
@@ -4533,7 +4533,7 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>31.975042,34.810956</t>
+          <t>31.980488,34.813327</t>
         </is>
       </c>
     </row>
@@ -4593,7 +4593,7 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>32.048554,34.814926</t>
+          <t>32.051929,34.814324</t>
         </is>
       </c>
     </row>
@@ -4617,7 +4617,7 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>31.897055,34.800408</t>
+          <t>31.893720,34.803882</t>
         </is>
       </c>
     </row>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.197179,34.956413</t>
         </is>
       </c>
     </row>
@@ -4701,7 +4701,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>32.151070,34.847113</t>
+          <t>32.153195,34.846595</t>
         </is>
       </c>
     </row>
@@ -4761,7 +4761,7 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>31.747225,35.212499</t>
+          <t>31.746771,35.212895</t>
         </is>
       </c>
     </row>
@@ -4773,7 +4773,7 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.197179,34.956413</t>
         </is>
       </c>
     </row>
@@ -4809,7 +4809,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>31.773929,34.629620</t>
+          <t>31.783743,34.661290</t>
         </is>
       </c>
     </row>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>31.755957,34.989832</t>
+          <t>31.755751,34.983774</t>
         </is>
       </c>
     </row>
@@ -4905,7 +4905,7 @@
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>31.784215,35.117210</t>
+          <t>31.767207,35.224441</t>
         </is>
       </c>
     </row>
@@ -4941,7 +4941,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>32.100120,34.828677</t>
+          <t>32.100317,34.828653</t>
         </is>
       </c>
     </row>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -5073,7 +5073,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -5085,7 +5085,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>32.165553,34.813406</t>
+          <t>32.166162,34.810351</t>
         </is>
       </c>
     </row>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>31.982527,34.765084</t>
+          <t>31.992690,34.909264</t>
         </is>
       </c>
     </row>
@@ -5133,7 +5133,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>31.807623,34.664804</t>
+          <t>31.813664,34.667678</t>
         </is>
       </c>
     </row>
@@ -5205,7 +5205,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>32.055436,34.805472</t>
+          <t>32.054678,34.804617</t>
         </is>
       </c>
     </row>
@@ -5229,7 +5229,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>32.020682,34.805150</t>
+          <t>32.011816,34.796993</t>
         </is>
       </c>
     </row>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>32.097022,34.829235</t>
+          <t>31.937727,34.837262</t>
         </is>
       </c>
     </row>
@@ -5265,7 +5265,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>31.665784,34.601137</t>
+          <t>31.663407,34.599960</t>
         </is>
       </c>
     </row>
@@ -5313,7 +5313,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>31.677567,34.596921</t>
+          <t>31.675767,34.597809</t>
         </is>
       </c>
     </row>
@@ -5349,7 +5349,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>31.946849,34.879864</t>
+          <t>31.942541,34.872538</t>
         </is>
       </c>
     </row>
@@ -5409,7 +5409,7 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>31.858484,35.215449</t>
+          <t>31.855315,35.221246</t>
         </is>
       </c>
     </row>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>31.750492,35.215772</t>
+          <t>31.750585,35.215673</t>
         </is>
       </c>
     </row>
@@ -5457,7 +5457,7 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>31.858484,35.215449</t>
+          <t>31.855315,35.221246</t>
         </is>
       </c>
     </row>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>31.792463,35.144323</t>
+          <t>31.792434,35.144275</t>
         </is>
       </c>
     </row>
@@ -5493,7 +5493,7 @@
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>31.753295,34.996429</t>
+          <t>31.755957,34.989832</t>
         </is>
       </c>
     </row>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>32.033552,34.851439</t>
+          <t>32.006200,34.743653</t>
         </is>
       </c>
     </row>
@@ -5553,7 +5553,7 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>31.225747,34.809580</t>
+          <t>31.226237,34.809557</t>
         </is>
       </c>
     </row>
@@ -5637,7 +5637,7 @@
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>31.862441,35.220615</t>
+          <t>31.860925,35.220821</t>
         </is>
       </c>
     </row>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>31.225747,34.809580</t>
+          <t>31.226237,34.809557</t>
         </is>
       </c>
     </row>
@@ -5721,7 +5721,7 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>31.223100,34.820208</t>
+          <t>31.222301,34.819116</t>
         </is>
       </c>
     </row>
@@ -5769,7 +5769,7 @@
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>32.171208,34.826985</t>
+          <t>32.167359,34.823770</t>
         </is>
       </c>
     </row>
@@ -5853,7 +5853,7 @@
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>31.226551,34.807177</t>
+          <t>31.226727,34.804803</t>
         </is>
       </c>
     </row>
@@ -5865,7 +5865,7 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>31.826014,34.658552</t>
+          <t>31.828293,34.662887</t>
         </is>
       </c>
     </row>
@@ -5889,7 +5889,7 @@
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>31.666206,34.591622</t>
+          <t>31.666065,34.584567</t>
         </is>
       </c>
     </row>
@@ -5913,7 +5913,7 @@
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>32.001232,34.801778</t>
+          <t>32.008568,34.807885</t>
         </is>
       </c>
     </row>
@@ -5925,7 +5925,7 @@
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>32.095724,34.858840</t>
+          <t>32.095945,34.859010</t>
         </is>
       </c>
     </row>
@@ -5937,7 +5937,7 @@
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>31.223512,34.880824</t>
+          <t>31.222537,34.880798</t>
         </is>
       </c>
     </row>
@@ -5949,7 +5949,7 @@
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>31.217089,34.816739</t>
+          <t>31.220502,34.815623</t>
         </is>
       </c>
     </row>
@@ -5997,7 +5997,7 @@
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>31.236692,34.796056</t>
+          <t>31.237729,34.793597</t>
         </is>
       </c>
     </row>
@@ -6009,7 +6009,7 @@
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>32.068716,34.778964</t>
+          <t>32.159475,34.836814</t>
         </is>
       </c>
     </row>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>32.107402,34.938858</t>
+          <t>32.108556,34.939938</t>
         </is>
       </c>
     </row>
@@ -6129,7 +6129,7 @@
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>31.665784,34.601137</t>
+          <t>31.663407,34.599960</t>
         </is>
       </c>
     </row>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -6225,7 +6225,7 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>32.047811,34.882122</t>
+          <t>31.526474,34.596970</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
refactored & reverted codebase to working state now includs ui changes for dailed coordinates and removed useless ui elements
</commit_message>
<xml_diff>
--- a/assets/api_detected_locations.xlsx
+++ b/assets/api_detected_locations.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>32.767884,34.966961</t>
+          <t>32.766882,34.967053</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>33.084756,35.112133</t>
+          <t>32.511729,35.502029</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.267628,34.993511</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>32.267628,34.993511</t>
+          <t>32.792761,34.995336</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>31.854920,35.218710</t>
+          <t>32.980490,35.542420</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>32.019045,34.841227</t>
+          <t>31.960770,34.876512</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.986934,35.708518</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>32.773251,35.044543</t>
+          <t>33.005860,35.094090</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>32.606459,35.290914</t>
+          <t>32.601426,35.289751</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>31.854920,35.218710</t>
+          <t>33.194459,35.572940</t>
         </is>
       </c>
     </row>
@@ -789,7 +789,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>31.961622,34.807607</t>
+          <t>31.961063,34.807761</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>32.035964,34.845985</t>
+          <t>32.036425,34.842884</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>31.977527,34.808252</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>31.767207,35.224441</t>
+          <t>31.784215,35.117210</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>32.052244,34.797643</t>
+          <t>32.058998,34.815227</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>32.047035,34.899314</t>
+          <t>32.121447,34.803699</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>31.818922,35.194455</t>
+          <t>32.692764,34.940222</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>32.234686,34.954455</t>
+          <t>32.775683,34.967878</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.199671,35.212911</t>
         </is>
       </c>
     </row>
@@ -945,7 +945,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>32.049544,34.764454</t>
+          <t>32.049533,34.764483</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>32.037040,34.776415</t>
+          <t>32.792761,34.995336</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>32.081982,34.816659</t>
+          <t>31.814560,34.779980</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>32.028209,34.802593</t>
+          <t>31.248833,35.198232</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>33.132610,35.690627</t>
+          <t>32.074578,34.805974</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>31.767207,35.224441</t>
+          <t>32.590574,34.936472</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>32.064156,34.854185</t>
+          <t>32.018460,34.748167</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>32.149836,34.846582</t>
+          <t>31.822668,35.253867</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>32.006200,34.743653</t>
+          <t>31.791658,34.651074</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>32.037040,34.776415</t>
+          <t>31.916670,35.016670</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>31.818922,35.194455</t>
+          <t>32.095980,34.774333</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>32.028209,34.802593</t>
+          <t>31.248833,35.198232</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>31.942541,34.872538</t>
+          <t>31.945204,34.878075</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>32.097875,34.896155</t>
+          <t>32.098181,34.896471</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>31.746015,35.213772</t>
+          <t>31.750898,35.207819</t>
         </is>
       </c>
     </row>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>31.194371,34.837706</t>
+          <t>32.177911,34.905656</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>31.748475,35.212194</t>
+          <t>32.049272,34.798714</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>32.174844,34.814576</t>
+          <t>32.009918,34.739188</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>31.785936,35.221741</t>
+          <t>31.314100,34.620250</t>
         </is>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>31.785077,34.693905</t>
+          <t>32.860863,35.099385</t>
         </is>
       </c>
     </row>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>31.977527,34.808252</t>
         </is>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>31.975998,34.882170</t>
+          <t>31.682230,34.745240</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>31.669726,34.779153</t>
+          <t>31.670900,34.779750</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>32.090535,34.885715</t>
+          <t>32.093309,34.885509</t>
         </is>
       </c>
     </row>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>32.063762,34.785644</t>
+          <t>32.447787,34.914428</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>31.767207,35.224441</t>
+          <t>32.696543,35.052512</t>
         </is>
       </c>
     </row>
@@ -2457,7 +2457,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>31.747674,35.214435</t>
+          <t>31.746624,35.213931</t>
         </is>
       </c>
     </row>
@@ -2541,7 +2541,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>32.823809,34.991295</t>
+          <t>32.819327,34.997607</t>
         </is>
       </c>
     </row>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>31.788356,35.213514</t>
+          <t>32.603829,35.298516</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>32.808325,35.060120</t>
+          <t>32.807619,35.057422</t>
         </is>
       </c>
     </row>
@@ -2649,7 +2649,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>32.806452,35.070911</t>
+          <t>32.804853,35.072857</t>
         </is>
       </c>
     </row>
@@ -2673,7 +2673,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>32.607513,35.292171</t>
+          <t>32.607430,35.292122</t>
         </is>
       </c>
     </row>
@@ -2685,7 +2685,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>32.787600,34.971328</t>
+          <t>32.782155,34.976622</t>
         </is>
       </c>
     </row>
@@ -2697,7 +2697,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>32.055436,34.805472</t>
+          <t>32.054678,34.804617</t>
         </is>
       </c>
     </row>
@@ -2769,7 +2769,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>32.818155,35.055460</t>
+          <t>32.815143,35.060720</t>
         </is>
       </c>
     </row>
@@ -2817,7 +2817,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>32.468029,34.974133</t>
+          <t>32.471755,34.969755</t>
         </is>
       </c>
     </row>
@@ -2889,7 +2889,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>32.209639,34.964653</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -2901,7 +2901,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>32.209639,34.964653</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>32.786982,35.518669</t>
+          <t>32.790077,35.516279</t>
         </is>
       </c>
     </row>
@@ -2961,7 +2961,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>32.142049,34.960396</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -2985,7 +2985,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>31.784988,35.210374</t>
+          <t>31.785087,35.210391</t>
         </is>
       </c>
     </row>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>32.142049,34.960396</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>32.927663,35.151740</t>
+          <t>32.916364,35.125162</t>
         </is>
       </c>
     </row>
@@ -3393,7 +3393,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>32.777112,35.040416</t>
+          <t>32.777129,35.040632</t>
         </is>
       </c>
     </row>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>32.634010,35.403998</t>
+          <t>32.854815,35.196680</t>
         </is>
       </c>
     </row>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>32.267628,34.993511</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>31.748498,35.214655</t>
+          <t>31.750585,35.215673</t>
         </is>
       </c>
     </row>
@@ -3633,7 +3633,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>31.750030,35.218672</t>
+          <t>31.750859,35.213920</t>
         </is>
       </c>
     </row>
@@ -3645,7 +3645,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>32.142049,34.960396</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>32.099723,34.828750</t>
+          <t>32.099592,34.828768</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>32.047831,34.870851</t>
+          <t>32.046554,34.869660</t>
         </is>
       </c>
     </row>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>32.983671,35.251911</t>
+          <t>32.984064,35.248787</t>
         </is>
       </c>
     </row>
@@ -3813,7 +3813,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>31.818001,34.669804</t>
+          <t>31.813664,34.667678</t>
         </is>
       </c>
     </row>
@@ -3825,7 +3825,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>31.667321,34.601532</t>
+          <t>31.663407,34.599960</t>
         </is>
       </c>
     </row>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>32.830002,34.970337</t>
+          <t>32.818629,34.996670</t>
         </is>
       </c>
     </row>
@@ -3969,7 +3969,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>31.748475,35.212194</t>
+          <t>31.750492,35.215772</t>
         </is>
       </c>
     </row>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>31.785263,35.186530</t>
+          <t>31.785775,35.182708</t>
         </is>
       </c>
     </row>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>31.748498,35.214655</t>
+          <t>31.750585,35.215673</t>
         </is>
       </c>
     </row>
@@ -4017,7 +4017,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>31.748475,35.212194</t>
+          <t>31.750492,35.215772</t>
         </is>
       </c>
     </row>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>32.193962,34.884145</t>
+          <t>32.194693,34.884294</t>
         </is>
       </c>
     </row>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>31.781986,35.164617</t>
+          <t>31.749963,35.141489</t>
         </is>
       </c>
     </row>
@@ -4173,7 +4173,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>33.003303,35.091469</t>
+          <t>33.003241,35.091790</t>
         </is>
       </c>
     </row>
@@ -4221,7 +4221,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>31.750030,35.218672</t>
+          <t>31.750859,35.213920</t>
         </is>
       </c>
     </row>
@@ -4449,7 +4449,7 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>32.956311,35.211352</t>
+          <t>32.949509,35.174243</t>
         </is>
       </c>
     </row>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>31.785087,35.210391</t>
+          <t>31.784988,35.210374</t>
         </is>
       </c>
     </row>
@@ -4509,7 +4509,7 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>31.758017,35.215239</t>
+          <t>31.757498,35.218264</t>
         </is>
       </c>
     </row>
@@ -4617,7 +4617,7 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>31.893720,34.803882</t>
+          <t>31.897055,34.800408</t>
         </is>
       </c>
     </row>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>32.142049,34.960396</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -4701,7 +4701,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>32.153195,34.846595</t>
+          <t>32.151070,34.847113</t>
         </is>
       </c>
     </row>
@@ -4725,7 +4725,7 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>33.230371,35.639263</t>
+          <t>31.652206,34.579598</t>
         </is>
       </c>
     </row>
@@ -4761,7 +4761,7 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>31.749399,35.210830</t>
+          <t>31.747225,35.212499</t>
         </is>
       </c>
     </row>
@@ -4809,7 +4809,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>32.798495,35.103304</t>
+          <t>31.773929,34.629620</t>
         </is>
       </c>
     </row>
@@ -4905,7 +4905,7 @@
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>31.767207,35.224441</t>
+          <t>31.784215,35.117210</t>
         </is>
       </c>
     </row>
@@ -4929,7 +4929,7 @@
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>32.149836,34.846582</t>
+          <t>32.151070,34.847113</t>
         </is>
       </c>
     </row>
@@ -4941,7 +4941,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>32.188320,34.866618</t>
+          <t>32.100120,34.828677</t>
         </is>
       </c>
     </row>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>32.267628,34.993511</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -5073,7 +5073,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>32.267628,34.993511</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -5085,7 +5085,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>32.166162,34.810351</t>
+          <t>32.165553,34.813406</t>
         </is>
       </c>
     </row>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>31.992690,34.909264</t>
+          <t>31.982527,34.765084</t>
         </is>
       </c>
     </row>
@@ -5133,7 +5133,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>32.189272,34.881159</t>
+          <t>31.807623,34.664804</t>
         </is>
       </c>
     </row>
@@ -5205,7 +5205,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>32.054678,34.804617</t>
+          <t>32.055436,34.805472</t>
         </is>
       </c>
     </row>
@@ -5229,7 +5229,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>31.785936,35.221741</t>
+          <t>32.020682,34.805150</t>
         </is>
       </c>
     </row>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>31.937727,34.837262</t>
+          <t>32.097022,34.829235</t>
         </is>
       </c>
     </row>
@@ -5265,7 +5265,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>31.663407,34.599960</t>
+          <t>31.665784,34.601137</t>
         </is>
       </c>
     </row>
@@ -5313,7 +5313,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>31.675767,34.597809</t>
+          <t>31.677567,34.596921</t>
         </is>
       </c>
     </row>
@@ -5349,7 +5349,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>31.942541,34.872538</t>
+          <t>31.946849,34.879864</t>
         </is>
       </c>
     </row>
@@ -5409,7 +5409,7 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>31.855315,35.221246</t>
+          <t>31.858484,35.215449</t>
         </is>
       </c>
     </row>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>31.750585,35.215673</t>
+          <t>31.750492,35.215772</t>
         </is>
       </c>
     </row>
@@ -5457,7 +5457,7 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>31.855315,35.221246</t>
+          <t>31.858484,35.215449</t>
         </is>
       </c>
     </row>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>32.086358,34.802173</t>
+          <t>31.792463,35.144323</t>
         </is>
       </c>
     </row>
@@ -5481,7 +5481,7 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>32.142049,34.960396</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -5505,7 +5505,7 @@
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>32.142049,34.960396</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -5541,7 +5541,7 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>31.238084,34.794545</t>
+          <t>31.238529,34.795441</t>
         </is>
       </c>
     </row>
@@ -5577,7 +5577,7 @@
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>32.142049,34.960396</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -5685,7 +5685,7 @@
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>31.669700,34.600713</t>
+          <t>31.319243,34.623672</t>
         </is>
       </c>
     </row>
@@ -5865,7 +5865,7 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>31.828282,34.663017</t>
+          <t>31.826014,34.658552</t>
         </is>
       </c>
     </row>
@@ -6057,7 +6057,7 @@
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>32.142049,34.960396</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>32.209639,34.964653</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -6189,7 +6189,7 @@
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>32.055436,34.805472</t>
+          <t>32.054678,34.804617</t>
         </is>
       </c>
     </row>
@@ -6225,7 +6225,7 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>31.526474,34.596970</t>
+          <t>32.047811,34.882122</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed visualization in optimization tab time limit = 5 minutes
</commit_message>
<xml_diff>
--- a/assets/api_detected_locations.xlsx
+++ b/assets/api_detected_locations.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>32.766882,34.967053</t>
+          <t>32.767884,34.966961</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>32.511729,35.502029</t>
+          <t>33.084756,35.112133</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>32.267628,34.993511</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>32.792761,34.995336</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>32.980490,35.542420</t>
+          <t>31.854920,35.218710</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>31.960770,34.876512</t>
+          <t>32.019045,34.841227</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>32.986934,35.708518</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>33.005860,35.094090</t>
+          <t>32.773251,35.044543</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>32.601426,35.289751</t>
+          <t>32.606459,35.290914</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>32.706861,35.173861</t>
+          <t>32.707298,35.173307</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>33.194459,35.572940</t>
+          <t>31.854920,35.218710</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>31.977527,34.808252</t>
+          <t>32.197179,34.956413</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>31.784215,35.117210</t>
+          <t>31.767207,35.224441</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>32.058998,34.815227</t>
+          <t>32.052244,34.797643</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>32.121447,34.803699</t>
+          <t>32.047035,34.899314</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>32.692764,34.940222</t>
+          <t>31.790191,35.198620</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>31.750585,35.215673</t>
+          <t>31.748498,35.214655</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>32.775683,34.967878</t>
+          <t>32.234686,34.954455</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>32.199671,35.212911</t>
+          <t>32.197179,34.956413</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>31.885539,34.789352</t>
+          <t>31.886326,34.786696</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>32.023189,34.796457</t>
+          <t>32.020531,34.799529</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>32.792761,34.995336</t>
+          <t>32.037040,34.776415</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>31.814560,34.779980</t>
+          <t>32.081982,34.816659</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>31.248833,35.198232</t>
+          <t>32.028209,34.802593</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>32.074578,34.805974</t>
+          <t>33.132610,35.690627</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>32.590574,34.936472</t>
+          <t>31.767207,35.224441</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>32.018460,34.748167</t>
+          <t>32.064156,34.854185</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>31.822668,35.253867</t>
+          <t>32.151070,34.847113</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>31.791658,34.651074</t>
+          <t>32.006200,34.743653</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>31.916670,35.016670</t>
+          <t>32.037040,34.776415</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>32.095980,34.774333</t>
+          <t>31.818922,35.194455</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>31.248833,35.198232</t>
+          <t>32.028209,34.802593</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>31.945204,34.878075</t>
+          <t>31.942541,34.872538</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>32.098181,34.896471</t>
+          <t>32.097875,34.896155</t>
         </is>
       </c>
     </row>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>32.177911,34.905656</t>
+          <t>31.194371,34.837706</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>32.049272,34.798714</t>
+          <t>31.748475,35.212194</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>32.009918,34.739188</t>
+          <t>32.174844,34.814576</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>31.314100,34.620250</t>
+          <t>31.785936,35.221741</t>
         </is>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>32.860863,35.099385</t>
+          <t>31.785077,34.693905</t>
         </is>
       </c>
     </row>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>31.977527,34.808252</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>31.682230,34.745240</t>
+          <t>31.975998,34.882170</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>31.670900,34.779750</t>
+          <t>31.669726,34.779153</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>32.093309,34.885509</t>
+          <t>32.090535,34.885715</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>32.807619,35.057422</t>
+          <t>32.783385,35.036378</t>
         </is>
       </c>
     </row>
@@ -2961,7 +2961,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>32.916364,35.125162</t>
+          <t>32.927663,35.151740</t>
         </is>
       </c>
     </row>
@@ -3393,7 +3393,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>32.777129,35.040632</t>
+          <t>32.777112,35.040416</t>
         </is>
       </c>
     </row>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.209639,34.964653</t>
         </is>
       </c>
     </row>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>31.750585,35.215673</t>
+          <t>31.748475,35.212194</t>
         </is>
       </c>
     </row>
@@ -3633,7 +3633,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>31.750859,35.213920</t>
+          <t>31.750030,35.218672</t>
         </is>
       </c>
     </row>
@@ -3645,7 +3645,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.197179,34.956413</t>
         </is>
       </c>
     </row>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>32.099592,34.828768</t>
+          <t>32.099723,34.828750</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>32.046554,34.869660</t>
+          <t>32.047831,34.870851</t>
         </is>
       </c>
     </row>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>32.984064,35.248787</t>
+          <t>32.983671,35.251911</t>
         </is>
       </c>
     </row>
@@ -3813,7 +3813,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>31.813664,34.667678</t>
+          <t>31.818001,34.669804</t>
         </is>
       </c>
     </row>
@@ -3825,7 +3825,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>31.663407,34.599960</t>
+          <t>31.667321,34.601532</t>
         </is>
       </c>
     </row>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>32.818629,34.996670</t>
+          <t>32.830002,34.970337</t>
         </is>
       </c>
     </row>
@@ -3969,7 +3969,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>31.750492,35.215772</t>
+          <t>31.748475,35.212194</t>
         </is>
       </c>
     </row>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>31.785775,35.182708</t>
+          <t>31.785263,35.186530</t>
         </is>
       </c>
     </row>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>31.750585,35.215673</t>
+          <t>31.748475,35.212194</t>
         </is>
       </c>
     </row>
@@ -4017,7 +4017,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>31.750492,35.215772</t>
+          <t>31.748475,35.212194</t>
         </is>
       </c>
     </row>
@@ -4041,7 +4041,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>31.750585,35.215673</t>
+          <t>31.748498,35.214655</t>
         </is>
       </c>
     </row>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>32.194693,34.884294</t>
+          <t>32.193962,34.884145</t>
         </is>
       </c>
     </row>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>31.749963,35.141489</t>
+          <t>31.781986,35.164617</t>
         </is>
       </c>
     </row>
@@ -4173,7 +4173,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>33.003241,35.091790</t>
+          <t>33.003303,35.091469</t>
         </is>
       </c>
     </row>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>31.784988,35.210374</t>
+          <t>31.785087,35.210391</t>
         </is>
       </c>
     </row>
@@ -4497,7 +4497,7 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>31.856088,35.216314</t>
+          <t>31.850998,35.218030</t>
         </is>
       </c>
     </row>
@@ -4509,7 +4509,7 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>31.757498,35.218264</t>
+          <t>31.757946,35.215351</t>
         </is>
       </c>
     </row>
@@ -4533,7 +4533,7 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>31.975042,34.810956</t>
+          <t>31.980488,34.813327</t>
         </is>
       </c>
     </row>
@@ -4593,7 +4593,7 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>32.048554,34.814926</t>
+          <t>32.051929,34.814324</t>
         </is>
       </c>
     </row>
@@ -4617,7 +4617,7 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>31.897055,34.800408</t>
+          <t>31.893720,34.803882</t>
         </is>
       </c>
     </row>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.197179,34.956413</t>
         </is>
       </c>
     </row>
@@ -4701,7 +4701,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>32.151070,34.847113</t>
+          <t>32.153195,34.846595</t>
         </is>
       </c>
     </row>
@@ -4761,7 +4761,7 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>31.747225,35.212499</t>
+          <t>31.746771,35.212895</t>
         </is>
       </c>
     </row>
@@ -4773,7 +4773,7 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.197179,34.956413</t>
         </is>
       </c>
     </row>
@@ -4809,7 +4809,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>31.773929,34.629620</t>
+          <t>31.783743,34.661290</t>
         </is>
       </c>
     </row>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>31.755957,34.989832</t>
+          <t>31.755751,34.983774</t>
         </is>
       </c>
     </row>
@@ -4905,7 +4905,7 @@
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>31.784215,35.117210</t>
+          <t>31.767207,35.224441</t>
         </is>
       </c>
     </row>
@@ -4941,7 +4941,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>32.100120,34.828677</t>
+          <t>32.100317,34.828653</t>
         </is>
       </c>
     </row>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -5073,7 +5073,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -5085,7 +5085,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>32.165553,34.813406</t>
+          <t>32.166162,34.810351</t>
         </is>
       </c>
     </row>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>31.982527,34.765084</t>
+          <t>31.992690,34.909264</t>
         </is>
       </c>
     </row>
@@ -5133,7 +5133,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>31.807623,34.664804</t>
+          <t>31.813664,34.667678</t>
         </is>
       </c>
     </row>
@@ -5205,7 +5205,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>32.055436,34.805472</t>
+          <t>32.054678,34.804617</t>
         </is>
       </c>
     </row>
@@ -5229,7 +5229,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>32.020682,34.805150</t>
+          <t>32.011816,34.796993</t>
         </is>
       </c>
     </row>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>32.097022,34.829235</t>
+          <t>31.937727,34.837262</t>
         </is>
       </c>
     </row>
@@ -5265,7 +5265,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>31.665784,34.601137</t>
+          <t>31.663407,34.599960</t>
         </is>
       </c>
     </row>
@@ -5313,7 +5313,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>31.677567,34.596921</t>
+          <t>31.675767,34.597809</t>
         </is>
       </c>
     </row>
@@ -5349,7 +5349,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>31.946849,34.879864</t>
+          <t>31.942541,34.872538</t>
         </is>
       </c>
     </row>
@@ -5409,7 +5409,7 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>31.858484,35.215449</t>
+          <t>31.855315,35.221246</t>
         </is>
       </c>
     </row>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>31.750492,35.215772</t>
+          <t>31.750585,35.215673</t>
         </is>
       </c>
     </row>
@@ -5457,7 +5457,7 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>31.858484,35.215449</t>
+          <t>31.855315,35.221246</t>
         </is>
       </c>
     </row>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>31.792463,35.144323</t>
+          <t>31.792434,35.144275</t>
         </is>
       </c>
     </row>
@@ -5493,7 +5493,7 @@
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>31.753295,34.996429</t>
+          <t>31.755957,34.989832</t>
         </is>
       </c>
     </row>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>32.033552,34.851439</t>
+          <t>32.006200,34.743653</t>
         </is>
       </c>
     </row>
@@ -5553,7 +5553,7 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>31.225747,34.809580</t>
+          <t>31.226237,34.809557</t>
         </is>
       </c>
     </row>
@@ -5637,7 +5637,7 @@
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>31.862441,35.220615</t>
+          <t>31.860925,35.220821</t>
         </is>
       </c>
     </row>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>31.225747,34.809580</t>
+          <t>31.226237,34.809557</t>
         </is>
       </c>
     </row>
@@ -5721,7 +5721,7 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>31.223100,34.820208</t>
+          <t>31.222301,34.819116</t>
         </is>
       </c>
     </row>
@@ -5769,7 +5769,7 @@
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>32.171208,34.826985</t>
+          <t>32.167359,34.823770</t>
         </is>
       </c>
     </row>
@@ -5853,7 +5853,7 @@
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>31.226551,34.807177</t>
+          <t>31.226727,34.804803</t>
         </is>
       </c>
     </row>
@@ -5865,7 +5865,7 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>31.826014,34.658552</t>
+          <t>31.828293,34.662887</t>
         </is>
       </c>
     </row>
@@ -5889,7 +5889,7 @@
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>31.666206,34.591622</t>
+          <t>31.666065,34.584567</t>
         </is>
       </c>
     </row>
@@ -5913,7 +5913,7 @@
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>32.001232,34.801778</t>
+          <t>32.008568,34.807885</t>
         </is>
       </c>
     </row>
@@ -5925,7 +5925,7 @@
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>32.095724,34.858840</t>
+          <t>32.095945,34.859010</t>
         </is>
       </c>
     </row>
@@ -5937,7 +5937,7 @@
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>31.223512,34.880824</t>
+          <t>31.222537,34.880798</t>
         </is>
       </c>
     </row>
@@ -5949,7 +5949,7 @@
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>31.217089,34.816739</t>
+          <t>31.220502,34.815623</t>
         </is>
       </c>
     </row>
@@ -5997,7 +5997,7 @@
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>31.236692,34.796056</t>
+          <t>31.237729,34.793597</t>
         </is>
       </c>
     </row>
@@ -6009,7 +6009,7 @@
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>32.068716,34.778964</t>
+          <t>32.159475,34.836814</t>
         </is>
       </c>
     </row>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>32.107402,34.938858</t>
+          <t>32.108556,34.939938</t>
         </is>
       </c>
     </row>
@@ -6129,7 +6129,7 @@
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>31.665784,34.601137</t>
+          <t>31.663407,34.599960</t>
         </is>
       </c>
     </row>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>32.139558,34.959151</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -6225,7 +6225,7 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>32.047811,34.882122</t>
+          <t>31.526474,34.596970</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
reverted to 23.1.26 commit 6888bc7
</commit_message>
<xml_diff>
--- a/assets/api_detected_locations.xlsx
+++ b/assets/api_detected_locations.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>32.767884,34.966961</t>
+          <t>32.766882,34.967053</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>33.084756,35.112133</t>
+          <t>32.511729,35.502029</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.267628,34.993511</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.792761,34.995336</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>31.854920,35.218710</t>
+          <t>32.980490,35.542420</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>32.019045,34.841227</t>
+          <t>31.960770,34.876512</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.986934,35.708518</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>32.773251,35.044543</t>
+          <t>33.005860,35.094090</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>32.606459,35.290914</t>
+          <t>32.601426,35.289751</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>32.707298,35.173307</t>
+          <t>32.706861,35.173861</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>31.854920,35.218710</t>
+          <t>33.194459,35.572940</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>32.197179,34.956413</t>
+          <t>31.977527,34.808252</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>31.767207,35.224441</t>
+          <t>31.784215,35.117210</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>32.052244,34.797643</t>
+          <t>32.058998,34.815227</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>32.047035,34.899314</t>
+          <t>32.121447,34.803699</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>31.790191,35.198620</t>
+          <t>32.692764,34.940222</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>31.748498,35.214655</t>
+          <t>31.750585,35.215673</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>32.234686,34.954455</t>
+          <t>32.775683,34.967878</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>32.197179,34.956413</t>
+          <t>32.199671,35.212911</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>31.886326,34.786696</t>
+          <t>31.885539,34.789352</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>32.020531,34.799529</t>
+          <t>32.023189,34.796457</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>32.037040,34.776415</t>
+          <t>32.792761,34.995336</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>32.081982,34.816659</t>
+          <t>31.814560,34.779980</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>32.028209,34.802593</t>
+          <t>31.248833,35.198232</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>33.132610,35.690627</t>
+          <t>32.074578,34.805974</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>31.767207,35.224441</t>
+          <t>32.590574,34.936472</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>32.064156,34.854185</t>
+          <t>32.018460,34.748167</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>32.151070,34.847113</t>
+          <t>31.822668,35.253867</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>32.006200,34.743653</t>
+          <t>31.791658,34.651074</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>32.037040,34.776415</t>
+          <t>31.916670,35.016670</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>31.818922,35.194455</t>
+          <t>32.095980,34.774333</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>32.028209,34.802593</t>
+          <t>31.248833,35.198232</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>31.942541,34.872538</t>
+          <t>31.945204,34.878075</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>32.097875,34.896155</t>
+          <t>32.098181,34.896471</t>
         </is>
       </c>
     </row>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>31.194371,34.837706</t>
+          <t>32.177911,34.905656</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>31.748475,35.212194</t>
+          <t>32.049272,34.798714</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>32.174844,34.814576</t>
+          <t>32.009918,34.739188</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>31.785936,35.221741</t>
+          <t>31.314100,34.620250</t>
         </is>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>31.785077,34.693905</t>
+          <t>32.860863,35.099385</t>
         </is>
       </c>
     </row>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>31.977527,34.808252</t>
         </is>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>31.975998,34.882170</t>
+          <t>31.682230,34.745240</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>31.669726,34.779153</t>
+          <t>31.670900,34.779750</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>32.090535,34.885715</t>
+          <t>32.093309,34.885509</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>32.783385,35.036378</t>
+          <t>32.807619,35.057422</t>
         </is>
       </c>
     </row>
@@ -2961,7 +2961,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>32.927663,35.151740</t>
+          <t>32.916364,35.125162</t>
         </is>
       </c>
     </row>
@@ -3393,7 +3393,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>32.777112,35.040416</t>
+          <t>32.777129,35.040632</t>
         </is>
       </c>
     </row>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>32.209639,34.964653</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>31.748475,35.212194</t>
+          <t>31.750585,35.215673</t>
         </is>
       </c>
     </row>
@@ -3633,7 +3633,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>31.750030,35.218672</t>
+          <t>31.750859,35.213920</t>
         </is>
       </c>
     </row>
@@ -3645,7 +3645,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>32.197179,34.956413</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>32.099723,34.828750</t>
+          <t>32.099592,34.828768</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>32.047831,34.870851</t>
+          <t>32.046554,34.869660</t>
         </is>
       </c>
     </row>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>32.983671,35.251911</t>
+          <t>32.984064,35.248787</t>
         </is>
       </c>
     </row>
@@ -3813,7 +3813,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>31.818001,34.669804</t>
+          <t>31.813664,34.667678</t>
         </is>
       </c>
     </row>
@@ -3825,7 +3825,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>31.667321,34.601532</t>
+          <t>31.663407,34.599960</t>
         </is>
       </c>
     </row>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>32.830002,34.970337</t>
+          <t>32.818629,34.996670</t>
         </is>
       </c>
     </row>
@@ -3969,7 +3969,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>31.748475,35.212194</t>
+          <t>31.750492,35.215772</t>
         </is>
       </c>
     </row>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>31.785263,35.186530</t>
+          <t>31.785775,35.182708</t>
         </is>
       </c>
     </row>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>31.748475,35.212194</t>
+          <t>31.750585,35.215673</t>
         </is>
       </c>
     </row>
@@ -4017,7 +4017,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>31.748475,35.212194</t>
+          <t>31.750492,35.215772</t>
         </is>
       </c>
     </row>
@@ -4041,7 +4041,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>31.748498,35.214655</t>
+          <t>31.750585,35.215673</t>
         </is>
       </c>
     </row>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>32.193962,34.884145</t>
+          <t>32.194693,34.884294</t>
         </is>
       </c>
     </row>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>31.781986,35.164617</t>
+          <t>31.749963,35.141489</t>
         </is>
       </c>
     </row>
@@ -4173,7 +4173,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>33.003303,35.091469</t>
+          <t>33.003241,35.091790</t>
         </is>
       </c>
     </row>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>31.785087,35.210391</t>
+          <t>31.784988,35.210374</t>
         </is>
       </c>
     </row>
@@ -4497,7 +4497,7 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>31.850998,35.218030</t>
+          <t>31.856088,35.216314</t>
         </is>
       </c>
     </row>
@@ -4509,7 +4509,7 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>31.757946,35.215351</t>
+          <t>31.757498,35.218264</t>
         </is>
       </c>
     </row>
@@ -4533,7 +4533,7 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>31.980488,34.813327</t>
+          <t>31.975042,34.810956</t>
         </is>
       </c>
     </row>
@@ -4593,7 +4593,7 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>32.051929,34.814324</t>
+          <t>32.048554,34.814926</t>
         </is>
       </c>
     </row>
@@ -4617,7 +4617,7 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>31.893720,34.803882</t>
+          <t>31.897055,34.800408</t>
         </is>
       </c>
     </row>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>32.197179,34.956413</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -4701,7 +4701,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>32.153195,34.846595</t>
+          <t>32.151070,34.847113</t>
         </is>
       </c>
     </row>
@@ -4761,7 +4761,7 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>31.746771,35.212895</t>
+          <t>31.747225,35.212499</t>
         </is>
       </c>
     </row>
@@ -4773,7 +4773,7 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>32.197179,34.956413</t>
+          <t>32.163217,34.961133</t>
         </is>
       </c>
     </row>
@@ -4809,7 +4809,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>31.783743,34.661290</t>
+          <t>31.773929,34.629620</t>
         </is>
       </c>
     </row>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>31.755751,34.983774</t>
+          <t>31.755957,34.989832</t>
         </is>
       </c>
     </row>
@@ -4905,7 +4905,7 @@
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>31.767207,35.224441</t>
+          <t>31.784215,35.117210</t>
         </is>
       </c>
     </row>
@@ -4941,7 +4941,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>32.100317,34.828653</t>
+          <t>32.100120,34.828677</t>
         </is>
       </c>
     </row>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -5073,7 +5073,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -5085,7 +5085,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>32.166162,34.810351</t>
+          <t>32.165553,34.813406</t>
         </is>
       </c>
     </row>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>31.992690,34.909264</t>
+          <t>31.982527,34.765084</t>
         </is>
       </c>
     </row>
@@ -5133,7 +5133,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>31.813664,34.667678</t>
+          <t>31.807623,34.664804</t>
         </is>
       </c>
     </row>
@@ -5205,7 +5205,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>32.054678,34.804617</t>
+          <t>32.055436,34.805472</t>
         </is>
       </c>
     </row>
@@ -5229,7 +5229,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>32.011816,34.796993</t>
+          <t>32.020682,34.805150</t>
         </is>
       </c>
     </row>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>31.937727,34.837262</t>
+          <t>32.097022,34.829235</t>
         </is>
       </c>
     </row>
@@ -5265,7 +5265,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>31.663407,34.599960</t>
+          <t>31.665784,34.601137</t>
         </is>
       </c>
     </row>
@@ -5313,7 +5313,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>31.675767,34.597809</t>
+          <t>31.677567,34.596921</t>
         </is>
       </c>
     </row>
@@ -5349,7 +5349,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>31.942541,34.872538</t>
+          <t>31.946849,34.879864</t>
         </is>
       </c>
     </row>
@@ -5409,7 +5409,7 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>31.855315,35.221246</t>
+          <t>31.858484,35.215449</t>
         </is>
       </c>
     </row>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>31.750585,35.215673</t>
+          <t>31.750492,35.215772</t>
         </is>
       </c>
     </row>
@@ -5457,7 +5457,7 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>31.855315,35.221246</t>
+          <t>31.858484,35.215449</t>
         </is>
       </c>
     </row>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>31.792434,35.144275</t>
+          <t>31.792463,35.144323</t>
         </is>
       </c>
     </row>
@@ -5493,7 +5493,7 @@
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>31.755957,34.989832</t>
+          <t>31.753295,34.996429</t>
         </is>
       </c>
     </row>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>32.006200,34.743653</t>
+          <t>32.033552,34.851439</t>
         </is>
       </c>
     </row>
@@ -5553,7 +5553,7 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>31.226237,34.809557</t>
+          <t>31.225747,34.809580</t>
         </is>
       </c>
     </row>
@@ -5637,7 +5637,7 @@
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>31.860925,35.220821</t>
+          <t>31.862441,35.220615</t>
         </is>
       </c>
     </row>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>31.226237,34.809557</t>
+          <t>31.225747,34.809580</t>
         </is>
       </c>
     </row>
@@ -5721,7 +5721,7 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>31.222301,34.819116</t>
+          <t>31.223100,34.820208</t>
         </is>
       </c>
     </row>
@@ -5769,7 +5769,7 @@
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>32.167359,34.823770</t>
+          <t>32.171208,34.826985</t>
         </is>
       </c>
     </row>
@@ -5853,7 +5853,7 @@
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>31.226727,34.804803</t>
+          <t>31.226551,34.807177</t>
         </is>
       </c>
     </row>
@@ -5865,7 +5865,7 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>31.828293,34.662887</t>
+          <t>31.826014,34.658552</t>
         </is>
       </c>
     </row>
@@ -5889,7 +5889,7 @@
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>31.666065,34.584567</t>
+          <t>31.666206,34.591622</t>
         </is>
       </c>
     </row>
@@ -5913,7 +5913,7 @@
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>32.008568,34.807885</t>
+          <t>32.001232,34.801778</t>
         </is>
       </c>
     </row>
@@ -5925,7 +5925,7 @@
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>32.095945,34.859010</t>
+          <t>32.095724,34.858840</t>
         </is>
       </c>
     </row>
@@ -5937,7 +5937,7 @@
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>31.222537,34.880798</t>
+          <t>31.223512,34.880824</t>
         </is>
       </c>
     </row>
@@ -5949,7 +5949,7 @@
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>31.220502,34.815623</t>
+          <t>31.217089,34.816739</t>
         </is>
       </c>
     </row>
@@ -5997,7 +5997,7 @@
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>31.237729,34.793597</t>
+          <t>31.236692,34.796056</t>
         </is>
       </c>
     </row>
@@ -6009,7 +6009,7 @@
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>32.159475,34.836814</t>
+          <t>32.068716,34.778964</t>
         </is>
       </c>
     </row>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>32.108556,34.939938</t>
+          <t>32.107402,34.938858</t>
         </is>
       </c>
     </row>
@@ -6129,7 +6129,7 @@
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>31.663407,34.599960</t>
+          <t>31.665784,34.601137</t>
         </is>
       </c>
     </row>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>32.163217,34.961133</t>
+          <t>32.139558,34.959151</t>
         </is>
       </c>
     </row>
@@ -6225,7 +6225,7 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>31.526474,34.596970</t>
+          <t>32.047811,34.882122</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
final spider web routes fallback implemented to do: update ui to exclude static route tab.
</commit_message>
<xml_diff>
--- a/assets/api_detected_locations.xlsx
+++ b/assets/api_detected_locations.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>32.766882,34.967053</t>
+          <t>32.767884,34.966961</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>32.511729,35.502029</t>
+          <t>33.084756,35.112133</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>32.792761,34.995336</t>
+          <t>32.128872,34.948863</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>32.980490,35.542420</t>
+          <t>31.854920,35.218710</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>31.960770,34.876512</t>
+          <t>32.019045,34.841227</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>32.986934,35.708518</t>
+          <t>32.267628,34.993511</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>33.005860,35.094090</t>
+          <t>32.773251,35.044543</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>32.601426,35.289751</t>
+          <t>32.606459,35.290914</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>33.194459,35.572940</t>
+          <t>31.854920,35.218710</t>
         </is>
       </c>
     </row>
@@ -789,7 +789,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>31.961063,34.807761</t>
+          <t>31.961622,34.807607</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>32.036425,34.842884</t>
+          <t>32.035964,34.845985</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>31.977527,34.808252</t>
+          <t>32.267628,34.993511</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>31.784215,35.117210</t>
+          <t>31.767207,35.224441</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>32.058998,34.815227</t>
+          <t>32.052244,34.797643</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>32.121447,34.803699</t>
+          <t>32.047035,34.899314</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>32.692764,34.940222</t>
+          <t>31.790191,35.198620</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>32.775683,34.967878</t>
+          <t>32.233023,34.950420</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>32.199671,35.212911</t>
+          <t>32.267628,34.993511</t>
         </is>
       </c>
     </row>
@@ -945,7 +945,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>32.049533,34.764483</t>
+          <t>32.049544,34.764454</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>32.792761,34.995336</t>
+          <t>32.037040,34.776415</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>31.814560,34.779980</t>
+          <t>32.081982,34.816659</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>31.248833,35.198232</t>
+          <t>32.028209,34.802593</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>32.074578,34.805974</t>
+          <t>33.132610,35.690627</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>32.590574,34.936472</t>
+          <t>31.767207,35.224441</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>32.018460,34.748167</t>
+          <t>32.064156,34.854185</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>31.822668,35.253867</t>
+          <t>32.153195,34.846595</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>31.791658,34.651074</t>
+          <t>32.006200,34.743653</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>31.916670,35.016670</t>
+          <t>32.037040,34.776415</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>32.095980,34.774333</t>
+          <t>31.790191,35.198620</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>31.248833,35.198232</t>
+          <t>32.028209,34.802593</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>31.945204,34.878075</t>
+          <t>31.944800,34.877389</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>32.098181,34.896471</t>
+          <t>32.099281,34.896845</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>31.755957,34.989832</t>
+          <t>31.755751,34.983774</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>31.750898,35.207819</t>
+          <t>31.750988,35.207798</t>
         </is>
       </c>
     </row>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>31.858601,35.215336</t>
+          <t>31.853707,35.217433</t>
         </is>
       </c>
     </row>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>32.177911,34.905656</t>
+          <t>31.194371,34.837706</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>32.049272,34.798714</t>
+          <t>31.750585,35.215673</t>
         </is>
       </c>
     </row>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>31.226237,34.809557</t>
+          <t>31.223027,34.809387</t>
         </is>
       </c>
     </row>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>31.068012,35.007848</t>
+          <t>31.065689,35.014440</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>31.238084,34.794545</t>
+          <t>31.241723,34.804322</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>32.009918,34.739188</t>
+          <t>32.174844,34.814576</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>31.863239,34.743120</t>
+          <t>31.864522,34.741564</t>
         </is>
       </c>
     </row>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>31.928344,34.878259</t>
+          <t>31.927646,34.878243</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>32.174304,34.930966</t>
+          <t>32.175016,34.928954</t>
         </is>
       </c>
     </row>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>32.045852,34.752438</t>
+          <t>32.045844,34.752383</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>31.314100,34.620250</t>
+          <t>31.785936,35.221741</t>
         </is>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>32.860863,35.099385</t>
+          <t>31.785077,34.693905</t>
         </is>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>32.471921,34.946694</t>
+          <t>32.472006,34.946602</t>
         </is>
       </c>
     </row>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>31.663407,34.599960</t>
+          <t>31.667321,34.601532</t>
         </is>
       </c>
     </row>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>31.977527,34.808252</t>
+          <t>32.267563,34.993779</t>
         </is>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>31.682230,34.745240</t>
+          <t>31.975998,34.882170</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>31.670900,34.779750</t>
+          <t>31.669726,34.779153</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>32.093309,34.885509</t>
+          <t>32.092353,34.885480</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>31.246177,34.808709</t>
+          <t>31.244467,34.807280</t>
         </is>
       </c>
     </row>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>31.756796,34.988601</t>
+          <t>31.757029,34.990864</t>
         </is>
       </c>
     </row>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>32.053920,34.770991</t>
+          <t>32.053835,34.771023</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Dynamic time horizon added for master routes via configurable multiplier; soft upper bound remains UI time. Route-name clustering service added with Gush Dan central helper; seeded OR-Tools solve with fallback. UI wires clustering seed into optimizer.
</commit_message>
<xml_diff>
--- a/assets/api_detected_locations.xlsx
+++ b/assets/api_detected_locations.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>32.767884,34.966961</t>
+          <t>32.766882,34.967053</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>33.084756,35.112133</t>
+          <t>32.511729,35.502029</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>32.128872,34.948863</t>
+          <t>32.792761,34.995336</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>31.854920,35.218710</t>
+          <t>32.980490,35.542420</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>32.019045,34.841227</t>
+          <t>31.960770,34.876512</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>32.267628,34.993511</t>
+          <t>32.986934,35.708518</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>32.773251,35.044543</t>
+          <t>33.005860,35.094090</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>32.606459,35.290914</t>
+          <t>32.601426,35.289751</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>31.854920,35.218710</t>
+          <t>33.194459,35.572940</t>
         </is>
       </c>
     </row>
@@ -789,7 +789,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>31.961622,34.807607</t>
+          <t>31.961063,34.807761</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>32.035964,34.845985</t>
+          <t>32.036425,34.842884</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>32.267628,34.993511</t>
+          <t>31.977527,34.808252</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>31.767207,35.224441</t>
+          <t>31.784215,35.117210</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>32.052244,34.797643</t>
+          <t>32.058998,34.815227</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>32.047035,34.899314</t>
+          <t>32.121447,34.803699</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>31.790191,35.198620</t>
+          <t>32.692764,34.940222</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>32.233023,34.950420</t>
+          <t>32.775683,34.967878</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>32.267628,34.993511</t>
+          <t>32.199671,35.212911</t>
         </is>
       </c>
     </row>
@@ -945,7 +945,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>32.049544,34.764454</t>
+          <t>32.049533,34.764483</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>32.037040,34.776415</t>
+          <t>32.792761,34.995336</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>32.081982,34.816659</t>
+          <t>31.814560,34.779980</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>32.028209,34.802593</t>
+          <t>31.248833,35.198232</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>33.132610,35.690627</t>
+          <t>32.074578,34.805974</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>31.767207,35.224441</t>
+          <t>32.590574,34.936472</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>32.064156,34.854185</t>
+          <t>32.018460,34.748167</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>32.153195,34.846595</t>
+          <t>31.822668,35.253867</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>32.006200,34.743653</t>
+          <t>31.791658,34.651074</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>32.037040,34.776415</t>
+          <t>31.916670,35.016670</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>31.790191,35.198620</t>
+          <t>32.095980,34.774333</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>32.028209,34.802593</t>
+          <t>31.248833,35.198232</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>31.944800,34.877389</t>
+          <t>31.945204,34.878075</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>32.099281,34.896845</t>
+          <t>32.098181,34.896471</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>31.755751,34.983774</t>
+          <t>31.755957,34.989832</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>31.750988,35.207798</t>
+          <t>31.750898,35.207819</t>
         </is>
       </c>
     </row>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>31.853707,35.217433</t>
+          <t>31.858601,35.215336</t>
         </is>
       </c>
     </row>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>31.194371,34.837706</t>
+          <t>32.177911,34.905656</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>31.750585,35.215673</t>
+          <t>32.049272,34.798714</t>
         </is>
       </c>
     </row>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>31.223027,34.809387</t>
+          <t>31.226237,34.809557</t>
         </is>
       </c>
     </row>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>31.065689,35.014440</t>
+          <t>31.068012,35.007848</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>31.241723,34.804322</t>
+          <t>31.238084,34.794545</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>32.174844,34.814576</t>
+          <t>32.009918,34.739188</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>31.864522,34.741564</t>
+          <t>31.863239,34.743120</t>
         </is>
       </c>
     </row>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>31.927646,34.878243</t>
+          <t>31.928344,34.878259</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>32.175016,34.928954</t>
+          <t>32.174304,34.930966</t>
         </is>
       </c>
     </row>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>32.045844,34.752383</t>
+          <t>32.045852,34.752438</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>31.785936,35.221741</t>
+          <t>31.314100,34.620250</t>
         </is>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>31.785077,34.693905</t>
+          <t>32.860863,35.099385</t>
         </is>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>32.472006,34.946602</t>
+          <t>32.471921,34.946694</t>
         </is>
       </c>
     </row>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>31.667321,34.601532</t>
+          <t>31.663407,34.599960</t>
         </is>
       </c>
     </row>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>32.267563,34.993779</t>
+          <t>31.977527,34.808252</t>
         </is>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>31.975998,34.882170</t>
+          <t>31.682230,34.745240</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>31.669726,34.779153</t>
+          <t>31.670900,34.779750</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>32.092353,34.885480</t>
+          <t>32.093309,34.885509</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>31.244467,34.807280</t>
+          <t>31.246177,34.808709</t>
         </is>
       </c>
     </row>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>31.757029,34.990864</t>
+          <t>31.756796,34.988601</t>
         </is>
       </c>
     </row>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>32.053835,34.771023</t>
+          <t>32.053920,34.770991</t>
         </is>
       </c>
     </row>

</xml_diff>